<commit_message>
Updates for pocono tires, upgrades and talent file
</commit_message>
<xml_diff>
--- a/SCNG2023/SCNG23.xlsx
+++ b/SCNG2023/SCNG23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\steamapps\common\rFactor 2\ModDev\Vehicles\SCNG2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD06C4C-0911-499F-8F6C-F7AF85C1D531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB8D03A-C552-4FC6-ABA1-61BFDCCDB140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8268" yWindow="3192" windowWidth="30492" windowHeight="18228" xr2:uid="{EFDCF2A9-BB19-41B3-9ABE-71F143890471}"/>
+    <workbookView xWindow="8376" yWindow="6048" windowWidth="33084" windowHeight="16680" firstSheet="31" activeTab="36" xr2:uid="{EFDCF2A9-BB19-41B3-9ABE-71F143890471}"/>
   </bookViews>
   <sheets>
     <sheet name="Track_Params" sheetId="2" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2978" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2968" uniqueCount="146">
   <si>
     <t>Track</t>
   </si>
@@ -885,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50797FCF-F199-4D71-97F5-D5996F6AED8E}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="T38" sqref="T38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2569,7 +2569,7 @@
         <v>56</v>
       </c>
       <c r="F36">
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="G36">
         <v>19.100000000000001</v>
@@ -31179,10 +31179,10 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0540CD-1BF0-4B90-AF20-E14B5D2FD58A}">
-  <dimension ref="A1:AJ46"/>
+  <dimension ref="A1:AB46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:W1048576"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1:AA1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31202,29 +31202,22 @@
     <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.21875" customWidth="1"/>
+    <col min="17" max="17" width="22" customWidth="1"/>
+    <col min="18" max="18" width="17.33203125" customWidth="1"/>
     <col min="19" max="19" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>64</v>
       </c>
@@ -31295,46 +31288,22 @@
         <v>19</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>3</v>
+        <v>90</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>103</v>
       </c>
@@ -31377,23 +31346,8 @@
       <c r="W2" t="s">
         <v>21</v>
       </c>
-      <c r="X2">
-        <v>51.878999999999998</v>
-      </c>
-      <c r="Y2">
-        <v>0.125</v>
-      </c>
-      <c r="Z2">
-        <v>51.878999999999998</v>
-      </c>
-      <c r="AA2">
-        <v>0.125</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>119</v>
       </c>
@@ -31442,23 +31396,8 @@
       <c r="W3" t="s">
         <v>21</v>
       </c>
-      <c r="X3">
-        <v>51.878999999999998</v>
-      </c>
-      <c r="Y3">
-        <v>0.125</v>
-      </c>
-      <c r="Z3">
-        <v>51.878999999999998</v>
-      </c>
-      <c r="AA3">
-        <v>0.125</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>120</v>
       </c>
@@ -31502,7 +31441,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>121</v>
       </c>
@@ -31546,7 +31485,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>98</v>
       </c>
@@ -31590,7 +31529,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>123</v>
       </c>
@@ -31634,7 +31573,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>113</v>
       </c>
@@ -31678,7 +31617,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>131</v>
       </c>
@@ -31722,7 +31661,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>126</v>
       </c>
@@ -31766,7 +31705,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>97</v>
       </c>
@@ -31810,7 +31749,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>137</v>
       </c>
@@ -31854,7 +31793,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>102</v>
       </c>
@@ -31898,7 +31837,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>110</v>
       </c>
@@ -31942,7 +31881,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>122</v>
       </c>
@@ -31986,7 +31925,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>129</v>
       </c>

</xml_diff>

<commit_message>
Working Martinsvville and Dover tires
</commit_message>
<xml_diff>
--- a/SCNG2023/SCNG23.xlsx
+++ b/SCNG2023/SCNG23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\rFactor 2\ModDev\Vehicles\SCNG2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B1EE0E-8244-4274-9855-94A8ECCBFAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228D6C62-AA5E-41D1-AA04-F923A3421533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35085" yWindow="3480" windowWidth="34725" windowHeight="16740" activeTab="5" xr2:uid="{EFDCF2A9-BB19-41B3-9ABE-71F143890471}"/>
+    <workbookView xWindow="-36495" yWindow="3165" windowWidth="34725" windowHeight="16740" firstSheet="11" activeTab="15" xr2:uid="{EFDCF2A9-BB19-41B3-9ABE-71F143890471}"/>
   </bookViews>
   <sheets>
     <sheet name="Track_Params" sheetId="2" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2969" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3051" uniqueCount="146">
   <si>
     <t>Track</t>
   </si>
@@ -7850,8 +7850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{031BC61E-D7E3-40D2-B13B-EEDD8447CE9B}">
   <dimension ref="A1:AB46"/>
   <sheetViews>
-    <sheetView topLeftCell="F12" workbookViewId="0">
-      <selection sqref="A1:W46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8008,6 +8008,9 @@
       <c r="Q2">
         <v>0.125</v>
       </c>
+      <c r="R2">
+        <v>22.44</v>
+      </c>
       <c r="S2">
         <v>0.125</v>
       </c>
@@ -8056,7 +8059,7 @@
         <v>0.125</v>
       </c>
       <c r="R3">
-        <v>31.2</v>
+        <v>22.44</v>
       </c>
       <c r="S3">
         <v>0.125</v>
@@ -8102,6 +8105,9 @@
       <c r="Q4">
         <v>0.125</v>
       </c>
+      <c r="R4">
+        <v>22.44</v>
+      </c>
       <c r="S4">
         <v>0.125</v>
       </c>
@@ -8146,6 +8152,9 @@
       <c r="Q5">
         <v>0.125</v>
       </c>
+      <c r="R5">
+        <v>22.44</v>
+      </c>
       <c r="S5">
         <v>0.125</v>
       </c>
@@ -8190,6 +8199,9 @@
       <c r="Q6">
         <v>0.125</v>
       </c>
+      <c r="R6">
+        <v>22.44</v>
+      </c>
       <c r="S6">
         <v>0.125</v>
       </c>
@@ -8234,6 +8246,9 @@
       <c r="Q7">
         <v>0.125</v>
       </c>
+      <c r="R7">
+        <v>22.5</v>
+      </c>
       <c r="S7">
         <v>0.125</v>
       </c>
@@ -8278,6 +8293,9 @@
       <c r="Q8">
         <v>0.125</v>
       </c>
+      <c r="R8">
+        <v>22.5</v>
+      </c>
       <c r="S8">
         <v>0.125</v>
       </c>
@@ -8322,6 +8340,9 @@
       <c r="Q9">
         <v>0.125</v>
       </c>
+      <c r="R9">
+        <v>22.5</v>
+      </c>
       <c r="S9">
         <v>0.125</v>
       </c>
@@ -8366,6 +8387,9 @@
       <c r="Q10">
         <v>0.125</v>
       </c>
+      <c r="R10">
+        <v>22.5</v>
+      </c>
       <c r="S10">
         <v>0.125</v>
       </c>
@@ -8410,6 +8434,9 @@
       <c r="Q11">
         <v>0.125</v>
       </c>
+      <c r="R11">
+        <v>22.6</v>
+      </c>
       <c r="S11">
         <v>0.125</v>
       </c>
@@ -8454,6 +8481,9 @@
       <c r="Q12">
         <v>0.125</v>
       </c>
+      <c r="R12">
+        <v>22.6</v>
+      </c>
       <c r="S12">
         <v>0.125</v>
       </c>
@@ -8498,6 +8528,9 @@
       <c r="Q13">
         <v>0.125</v>
       </c>
+      <c r="R13">
+        <v>22.6</v>
+      </c>
       <c r="S13">
         <v>0.125</v>
       </c>
@@ -8542,6 +8575,9 @@
       <c r="Q14">
         <v>0.125</v>
       </c>
+      <c r="R14">
+        <v>22.7</v>
+      </c>
       <c r="S14">
         <v>0.125</v>
       </c>
@@ -8586,6 +8622,9 @@
       <c r="Q15">
         <v>0.125</v>
       </c>
+      <c r="R15">
+        <v>22.7</v>
+      </c>
       <c r="S15">
         <v>0.125</v>
       </c>
@@ -8630,6 +8669,9 @@
       <c r="Q16">
         <v>0.125</v>
       </c>
+      <c r="R16">
+        <v>22.7</v>
+      </c>
       <c r="S16">
         <v>0.125</v>
       </c>
@@ -8674,6 +8716,9 @@
       <c r="Q17">
         <v>0.125</v>
       </c>
+      <c r="R17">
+        <v>22.7</v>
+      </c>
       <c r="S17">
         <v>0.125</v>
       </c>
@@ -8718,6 +8763,9 @@
       <c r="Q18">
         <v>0.125</v>
       </c>
+      <c r="R18">
+        <v>22.7</v>
+      </c>
       <c r="S18">
         <v>0.125</v>
       </c>
@@ -8762,6 +8810,9 @@
       <c r="Q19">
         <v>0.125</v>
       </c>
+      <c r="R19">
+        <v>22.7</v>
+      </c>
       <c r="S19">
         <v>0.125</v>
       </c>
@@ -8806,6 +8857,9 @@
       <c r="Q20">
         <v>0.125</v>
       </c>
+      <c r="R20">
+        <v>22.7</v>
+      </c>
       <c r="S20">
         <v>0.125</v>
       </c>
@@ -8850,6 +8904,9 @@
       <c r="Q21">
         <v>0.125</v>
       </c>
+      <c r="R21">
+        <v>22.7</v>
+      </c>
       <c r="S21">
         <v>0.125</v>
       </c>
@@ -8893,6 +8950,9 @@
       </c>
       <c r="Q22">
         <v>0.125</v>
+      </c>
+      <c r="R22">
+        <v>22.8</v>
       </c>
       <c r="S22">
         <v>0.125</v>
@@ -8938,6 +8998,9 @@
       <c r="Q23">
         <v>0.125</v>
       </c>
+      <c r="R23">
+        <v>22.8</v>
+      </c>
       <c r="S23">
         <v>0.125</v>
       </c>
@@ -8982,6 +9045,9 @@
       <c r="Q24">
         <v>0.125</v>
       </c>
+      <c r="R24">
+        <v>22.8</v>
+      </c>
       <c r="S24">
         <v>0.125</v>
       </c>
@@ -9026,6 +9092,9 @@
       <c r="Q25">
         <v>0.125</v>
       </c>
+      <c r="R25">
+        <v>22.9</v>
+      </c>
       <c r="S25">
         <v>0.125</v>
       </c>
@@ -9070,6 +9139,9 @@
       <c r="Q26">
         <v>0.125</v>
       </c>
+      <c r="R26">
+        <v>22.9</v>
+      </c>
       <c r="S26">
         <v>0.125</v>
       </c>
@@ -9114,6 +9186,9 @@
       <c r="Q27">
         <v>0.125</v>
       </c>
+      <c r="R27">
+        <v>23</v>
+      </c>
       <c r="S27">
         <v>0.125</v>
       </c>
@@ -9158,6 +9233,9 @@
       <c r="Q28">
         <v>0.125</v>
       </c>
+      <c r="R28">
+        <v>23</v>
+      </c>
       <c r="S28">
         <v>0.125</v>
       </c>
@@ -9202,6 +9280,9 @@
       <c r="Q29">
         <v>0.125</v>
       </c>
+      <c r="R29">
+        <v>23</v>
+      </c>
       <c r="S29">
         <v>0.125</v>
       </c>
@@ -9246,6 +9327,9 @@
       <c r="Q30">
         <v>0.125</v>
       </c>
+      <c r="R30">
+        <v>23</v>
+      </c>
       <c r="S30">
         <v>0.125</v>
       </c>
@@ -9290,6 +9374,9 @@
       <c r="Q31">
         <v>0.125</v>
       </c>
+      <c r="R31">
+        <v>23</v>
+      </c>
       <c r="S31">
         <v>0.125</v>
       </c>
@@ -9334,6 +9421,9 @@
       <c r="Q32">
         <v>0.125</v>
       </c>
+      <c r="R32">
+        <v>23</v>
+      </c>
       <c r="S32">
         <v>0.125</v>
       </c>
@@ -9378,6 +9468,9 @@
       <c r="Q33">
         <v>0.125</v>
       </c>
+      <c r="R33">
+        <v>23</v>
+      </c>
       <c r="S33">
         <v>0.125</v>
       </c>
@@ -9422,6 +9515,9 @@
       <c r="Q34">
         <v>0.125</v>
       </c>
+      <c r="R34">
+        <v>23</v>
+      </c>
       <c r="S34">
         <v>0.125</v>
       </c>
@@ -9466,6 +9562,9 @@
       <c r="Q35">
         <v>0.125</v>
       </c>
+      <c r="R35">
+        <v>23</v>
+      </c>
       <c r="S35">
         <v>0.125</v>
       </c>
@@ -9510,6 +9609,9 @@
       <c r="Q36">
         <v>0.125</v>
       </c>
+      <c r="R36">
+        <v>23.2</v>
+      </c>
       <c r="S36">
         <v>0.125</v>
       </c>
@@ -9554,6 +9656,9 @@
       <c r="Q37">
         <v>0.125</v>
       </c>
+      <c r="R37">
+        <v>23.2</v>
+      </c>
       <c r="S37">
         <v>0.125</v>
       </c>
@@ -9598,6 +9703,9 @@
       <c r="Q38">
         <v>0.125</v>
       </c>
+      <c r="R38">
+        <v>23.2</v>
+      </c>
       <c r="S38">
         <v>0.125</v>
       </c>
@@ -9642,6 +9750,9 @@
       <c r="Q39">
         <v>0.125</v>
       </c>
+      <c r="R39">
+        <v>23.3</v>
+      </c>
       <c r="S39">
         <v>0.125</v>
       </c>
@@ -9686,6 +9797,9 @@
       <c r="Q40">
         <v>0.125</v>
       </c>
+      <c r="R40">
+        <v>23.3</v>
+      </c>
       <c r="S40">
         <v>0.125</v>
       </c>
@@ -9734,7 +9848,7 @@
         <v>0.125</v>
       </c>
       <c r="R41">
-        <v>31.3</v>
+        <v>23.3</v>
       </c>
       <c r="S41">
         <v>0.125</v>
@@ -9780,6 +9894,9 @@
       <c r="Q42">
         <v>0.125</v>
       </c>
+      <c r="R42">
+        <v>23.3</v>
+      </c>
       <c r="S42">
         <v>0.125</v>
       </c>
@@ -9824,6 +9941,9 @@
       <c r="Q43">
         <v>0.125</v>
       </c>
+      <c r="R43">
+        <v>23.3</v>
+      </c>
       <c r="S43">
         <v>0.125</v>
       </c>
@@ -9868,6 +9988,9 @@
       <c r="Q44">
         <v>0.125</v>
       </c>
+      <c r="R44">
+        <v>23.4</v>
+      </c>
       <c r="S44">
         <v>0.125</v>
       </c>
@@ -9912,6 +10035,9 @@
       <c r="Q45">
         <v>0.125</v>
       </c>
+      <c r="R45">
+        <v>23.4</v>
+      </c>
       <c r="S45">
         <v>0.125</v>
       </c>
@@ -9955,6 +10081,9 @@
       </c>
       <c r="Q46">
         <v>0.125</v>
+      </c>
+      <c r="R46">
+        <v>23.5</v>
       </c>
       <c r="S46">
         <v>0.125</v>
@@ -20059,170 +20188,10 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A64D242F-A9A5-4B1B-8CD5-C30FB8A11766}">
-  <dimension ref="A1:AJ1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="21.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D680271-2F3F-4CF6-9B65-8CE1BE598F0F}">
   <dimension ref="A1:AB46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20379,6 +20348,9 @@
       <c r="Q2">
         <v>0.125</v>
       </c>
+      <c r="R2">
+        <v>19.718</v>
+      </c>
       <c r="S2">
         <v>0.125</v>
       </c>
@@ -20397,7 +20369,7 @@
         <v>99</v>
       </c>
       <c r="D3">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E3">
         <v>99</v>
@@ -20427,7 +20399,7 @@
         <v>0.125</v>
       </c>
       <c r="R3">
-        <v>31.2</v>
+        <v>19.719000000000001</v>
       </c>
       <c r="S3">
         <v>0.125</v>
@@ -20447,7 +20419,7 @@
         <v>92</v>
       </c>
       <c r="D4">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E4">
         <v>90</v>
@@ -20472,6 +20444,9 @@
       </c>
       <c r="Q4">
         <v>0.125</v>
+      </c>
+      <c r="R4">
+        <v>19.725000000000001</v>
       </c>
       <c r="S4">
         <v>0.125</v>
@@ -20517,6 +20492,9 @@
       <c r="Q5">
         <v>0.125</v>
       </c>
+      <c r="R5">
+        <v>19.73</v>
+      </c>
       <c r="S5">
         <v>0.125</v>
       </c>
@@ -20561,6 +20539,9 @@
       <c r="Q6">
         <v>0.125</v>
       </c>
+      <c r="R6">
+        <v>19.73</v>
+      </c>
       <c r="S6">
         <v>0.125</v>
       </c>
@@ -20579,7 +20560,7 @@
         <v>92</v>
       </c>
       <c r="D7">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E7">
         <v>88</v>
@@ -20604,6 +20585,9 @@
       </c>
       <c r="Q7">
         <v>0.125</v>
+      </c>
+      <c r="R7">
+        <v>19.73</v>
       </c>
       <c r="S7">
         <v>0.125</v>
@@ -20649,6 +20633,9 @@
       <c r="Q8">
         <v>0.125</v>
       </c>
+      <c r="R8">
+        <v>19.73</v>
+      </c>
       <c r="S8">
         <v>0.125</v>
       </c>
@@ -20693,6 +20680,9 @@
       <c r="Q9">
         <v>0.125</v>
       </c>
+      <c r="R9">
+        <v>19.73</v>
+      </c>
       <c r="S9">
         <v>0.125</v>
       </c>
@@ -20737,6 +20727,9 @@
       <c r="Q10">
         <v>0.125</v>
       </c>
+      <c r="R10">
+        <v>19.73</v>
+      </c>
       <c r="S10">
         <v>0.125</v>
       </c>
@@ -20781,6 +20774,9 @@
       <c r="Q11">
         <v>0.125</v>
       </c>
+      <c r="R11">
+        <v>19.73</v>
+      </c>
       <c r="S11">
         <v>0.125</v>
       </c>
@@ -20825,6 +20821,9 @@
       <c r="Q12">
         <v>0.125</v>
       </c>
+      <c r="R12">
+        <v>19.73</v>
+      </c>
       <c r="S12">
         <v>0.125</v>
       </c>
@@ -20869,6 +20868,9 @@
       <c r="Q13">
         <v>0.125</v>
       </c>
+      <c r="R13">
+        <v>19.73</v>
+      </c>
       <c r="S13">
         <v>0.125</v>
       </c>
@@ -20913,6 +20915,9 @@
       <c r="Q14">
         <v>0.125</v>
       </c>
+      <c r="R14">
+        <v>19.850000000000001</v>
+      </c>
       <c r="S14">
         <v>0.125</v>
       </c>
@@ -20957,6 +20962,9 @@
       <c r="Q15">
         <v>0.125</v>
       </c>
+      <c r="R15">
+        <v>19.850000000000001</v>
+      </c>
       <c r="S15">
         <v>0.125</v>
       </c>
@@ -21001,6 +21009,9 @@
       <c r="Q16">
         <v>0.125</v>
       </c>
+      <c r="R16">
+        <v>19.850000000000001</v>
+      </c>
       <c r="S16">
         <v>0.125</v>
       </c>
@@ -21045,6 +21056,9 @@
       <c r="Q17">
         <v>0.125</v>
       </c>
+      <c r="R17">
+        <v>19.850000000000001</v>
+      </c>
       <c r="S17">
         <v>0.125</v>
       </c>
@@ -21089,6 +21103,9 @@
       <c r="Q18">
         <v>0.125</v>
       </c>
+      <c r="R18">
+        <v>19.850000000000001</v>
+      </c>
       <c r="S18">
         <v>0.125</v>
       </c>
@@ -21133,6 +21150,9 @@
       <c r="Q19">
         <v>0.125</v>
       </c>
+      <c r="R19">
+        <v>19.850000000000001</v>
+      </c>
       <c r="S19">
         <v>0.125</v>
       </c>
@@ -21177,6 +21197,9 @@
       <c r="Q20">
         <v>0.125</v>
       </c>
+      <c r="R20">
+        <v>19.850000000000001</v>
+      </c>
       <c r="S20">
         <v>0.125</v>
       </c>
@@ -21221,6 +21244,9 @@
       <c r="Q21">
         <v>0.125</v>
       </c>
+      <c r="R21">
+        <v>19.850000000000001</v>
+      </c>
       <c r="S21">
         <v>0.125</v>
       </c>
@@ -21264,6 +21290,9 @@
       </c>
       <c r="Q22">
         <v>0.125</v>
+      </c>
+      <c r="R22">
+        <v>19.850000000000001</v>
       </c>
       <c r="S22">
         <v>0.125</v>
@@ -21309,6 +21338,9 @@
       <c r="Q23">
         <v>0.125</v>
       </c>
+      <c r="R23">
+        <v>19.850000000000001</v>
+      </c>
       <c r="S23">
         <v>0.125</v>
       </c>
@@ -21353,6 +21385,9 @@
       <c r="Q24">
         <v>0.125</v>
       </c>
+      <c r="R24">
+        <v>19.850000000000001</v>
+      </c>
       <c r="S24">
         <v>0.125</v>
       </c>
@@ -21397,6 +21432,9 @@
       <c r="Q25">
         <v>0.125</v>
       </c>
+      <c r="R25">
+        <v>19.93</v>
+      </c>
       <c r="S25">
         <v>0.125</v>
       </c>
@@ -21441,6 +21479,9 @@
       <c r="Q26">
         <v>0.125</v>
       </c>
+      <c r="R26">
+        <v>19.93</v>
+      </c>
       <c r="S26">
         <v>0.125</v>
       </c>
@@ -21485,6 +21526,9 @@
       <c r="Q27">
         <v>0.125</v>
       </c>
+      <c r="R27">
+        <v>19.93</v>
+      </c>
       <c r="S27">
         <v>0.125</v>
       </c>
@@ -21529,6 +21573,9 @@
       <c r="Q28">
         <v>0.125</v>
       </c>
+      <c r="R28">
+        <v>19.93</v>
+      </c>
       <c r="S28">
         <v>0.125</v>
       </c>
@@ -21573,6 +21620,9 @@
       <c r="Q29">
         <v>0.125</v>
       </c>
+      <c r="R29">
+        <v>19.93</v>
+      </c>
       <c r="S29">
         <v>0.125</v>
       </c>
@@ -21617,6 +21667,9 @@
       <c r="Q30">
         <v>0.125</v>
       </c>
+      <c r="R30">
+        <v>19.93</v>
+      </c>
       <c r="S30">
         <v>0.125</v>
       </c>
@@ -21661,6 +21714,9 @@
       <c r="Q31">
         <v>0.125</v>
       </c>
+      <c r="R31">
+        <v>19.93</v>
+      </c>
       <c r="S31">
         <v>0.125</v>
       </c>
@@ -21705,6 +21761,9 @@
       <c r="Q32">
         <v>0.125</v>
       </c>
+      <c r="R32">
+        <v>19.93</v>
+      </c>
       <c r="S32">
         <v>0.125</v>
       </c>
@@ -21749,6 +21808,9 @@
       <c r="Q33">
         <v>0.125</v>
       </c>
+      <c r="R33">
+        <v>20</v>
+      </c>
       <c r="S33">
         <v>0.125</v>
       </c>
@@ -21793,6 +21855,9 @@
       <c r="Q34">
         <v>0.125</v>
       </c>
+      <c r="R34">
+        <v>20</v>
+      </c>
       <c r="S34">
         <v>0.125</v>
       </c>
@@ -21837,6 +21902,9 @@
       <c r="Q35">
         <v>0.125</v>
       </c>
+      <c r="R35">
+        <v>20</v>
+      </c>
       <c r="S35">
         <v>0.125</v>
       </c>
@@ -21881,6 +21949,9 @@
       <c r="Q36">
         <v>0.125</v>
       </c>
+      <c r="R36">
+        <v>20</v>
+      </c>
       <c r="S36">
         <v>0.125</v>
       </c>
@@ -21925,6 +21996,9 @@
       <c r="Q37">
         <v>0.125</v>
       </c>
+      <c r="R37">
+        <v>20</v>
+      </c>
       <c r="S37">
         <v>0.125</v>
       </c>
@@ -21969,6 +22043,9 @@
       <c r="Q38">
         <v>0.125</v>
       </c>
+      <c r="R38">
+        <v>20</v>
+      </c>
       <c r="S38">
         <v>0.125</v>
       </c>
@@ -22013,6 +22090,9 @@
       <c r="Q39">
         <v>0.125</v>
       </c>
+      <c r="R39">
+        <v>20</v>
+      </c>
       <c r="S39">
         <v>0.125</v>
       </c>
@@ -22057,6 +22137,9 @@
       <c r="Q40">
         <v>0.125</v>
       </c>
+      <c r="R40">
+        <v>20.100000000000001</v>
+      </c>
       <c r="S40">
         <v>0.125</v>
       </c>
@@ -22105,7 +22188,7 @@
         <v>0.125</v>
       </c>
       <c r="R41">
-        <v>31.3</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="S41">
         <v>0.125</v>
@@ -22151,6 +22234,9 @@
       <c r="Q42">
         <v>0.125</v>
       </c>
+      <c r="R42">
+        <v>20.2</v>
+      </c>
       <c r="S42">
         <v>0.125</v>
       </c>
@@ -22195,6 +22281,9 @@
       <c r="Q43">
         <v>0.125</v>
       </c>
+      <c r="R43">
+        <v>20.2</v>
+      </c>
       <c r="S43">
         <v>0.125</v>
       </c>
@@ -22239,6 +22328,9 @@
       <c r="Q44">
         <v>0.125</v>
       </c>
+      <c r="R44">
+        <v>20.3</v>
+      </c>
       <c r="S44">
         <v>0.125</v>
       </c>
@@ -22283,6 +22375,9 @@
       <c r="Q45">
         <v>0.125</v>
       </c>
+      <c r="R45">
+        <v>20.3</v>
+      </c>
       <c r="S45">
         <v>0.125</v>
       </c>
@@ -22326,6 +22421,2260 @@
       </c>
       <c r="Q46">
         <v>0.125</v>
+      </c>
+      <c r="R46">
+        <v>20.3</v>
+      </c>
+      <c r="S46">
+        <v>0.125</v>
+      </c>
+      <c r="W46" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D680271-2F3F-4CF6-9B65-8CE1BE598F0F}">
+  <dimension ref="A1:AB46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>99</v>
+      </c>
+      <c r="D2">
+        <v>99</v>
+      </c>
+      <c r="E2">
+        <v>99</v>
+      </c>
+      <c r="F2">
+        <v>65</v>
+      </c>
+      <c r="G2">
+        <v>99</v>
+      </c>
+      <c r="H2">
+        <v>99</v>
+      </c>
+      <c r="J2">
+        <v>99</v>
+      </c>
+      <c r="M2">
+        <v>50</v>
+      </c>
+      <c r="N2">
+        <v>99</v>
+      </c>
+      <c r="Q2">
+        <v>0.125</v>
+      </c>
+      <c r="R2">
+        <v>19.718</v>
+      </c>
+      <c r="S2">
+        <v>0.125</v>
+      </c>
+      <c r="W2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>99</v>
+      </c>
+      <c r="D3">
+        <v>95</v>
+      </c>
+      <c r="E3">
+        <v>99</v>
+      </c>
+      <c r="F3">
+        <v>65</v>
+      </c>
+      <c r="G3">
+        <v>99</v>
+      </c>
+      <c r="H3">
+        <v>99</v>
+      </c>
+      <c r="J3">
+        <v>99</v>
+      </c>
+      <c r="M3">
+        <v>50</v>
+      </c>
+      <c r="N3">
+        <v>99</v>
+      </c>
+      <c r="P3">
+        <v>31.2</v>
+      </c>
+      <c r="Q3">
+        <v>0.125</v>
+      </c>
+      <c r="R3">
+        <v>19.719000000000001</v>
+      </c>
+      <c r="S3">
+        <v>0.125</v>
+      </c>
+      <c r="W3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>92</v>
+      </c>
+      <c r="D4">
+        <v>92</v>
+      </c>
+      <c r="E4">
+        <v>90</v>
+      </c>
+      <c r="F4">
+        <v>65</v>
+      </c>
+      <c r="G4">
+        <v>85</v>
+      </c>
+      <c r="H4">
+        <v>99</v>
+      </c>
+      <c r="J4">
+        <v>99</v>
+      </c>
+      <c r="M4">
+        <v>50</v>
+      </c>
+      <c r="N4">
+        <v>99</v>
+      </c>
+      <c r="Q4">
+        <v>0.125</v>
+      </c>
+      <c r="R4">
+        <v>19.725000000000001</v>
+      </c>
+      <c r="S4">
+        <v>0.125</v>
+      </c>
+      <c r="W4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>93</v>
+      </c>
+      <c r="D5">
+        <v>92</v>
+      </c>
+      <c r="E5">
+        <v>85</v>
+      </c>
+      <c r="F5">
+        <v>65</v>
+      </c>
+      <c r="G5">
+        <v>85</v>
+      </c>
+      <c r="H5">
+        <v>99</v>
+      </c>
+      <c r="J5">
+        <v>99</v>
+      </c>
+      <c r="M5">
+        <v>50</v>
+      </c>
+      <c r="N5">
+        <v>99</v>
+      </c>
+      <c r="Q5">
+        <v>0.125</v>
+      </c>
+      <c r="R5">
+        <v>19.73</v>
+      </c>
+      <c r="S5">
+        <v>0.125</v>
+      </c>
+      <c r="W5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>99</v>
+      </c>
+      <c r="D6">
+        <v>90</v>
+      </c>
+      <c r="E6">
+        <v>90</v>
+      </c>
+      <c r="F6">
+        <v>65</v>
+      </c>
+      <c r="G6">
+        <v>85</v>
+      </c>
+      <c r="H6">
+        <v>99</v>
+      </c>
+      <c r="J6">
+        <v>99</v>
+      </c>
+      <c r="M6">
+        <v>50</v>
+      </c>
+      <c r="N6">
+        <v>99</v>
+      </c>
+      <c r="Q6">
+        <v>0.125</v>
+      </c>
+      <c r="R6">
+        <v>19.73</v>
+      </c>
+      <c r="S6">
+        <v>0.125</v>
+      </c>
+      <c r="W6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>92</v>
+      </c>
+      <c r="D7">
+        <v>90</v>
+      </c>
+      <c r="E7">
+        <v>88</v>
+      </c>
+      <c r="F7">
+        <v>65</v>
+      </c>
+      <c r="G7">
+        <v>85</v>
+      </c>
+      <c r="H7">
+        <v>99</v>
+      </c>
+      <c r="J7">
+        <v>99</v>
+      </c>
+      <c r="M7">
+        <v>50</v>
+      </c>
+      <c r="N7">
+        <v>99</v>
+      </c>
+      <c r="Q7">
+        <v>0.125</v>
+      </c>
+      <c r="R7">
+        <v>19.73</v>
+      </c>
+      <c r="S7">
+        <v>0.125</v>
+      </c>
+      <c r="W7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>97</v>
+      </c>
+      <c r="D8">
+        <v>97</v>
+      </c>
+      <c r="E8">
+        <v>90</v>
+      </c>
+      <c r="F8">
+        <v>65</v>
+      </c>
+      <c r="G8">
+        <v>85</v>
+      </c>
+      <c r="H8">
+        <v>99</v>
+      </c>
+      <c r="J8">
+        <v>99</v>
+      </c>
+      <c r="M8">
+        <v>50</v>
+      </c>
+      <c r="N8">
+        <v>99</v>
+      </c>
+      <c r="Q8">
+        <v>0.125</v>
+      </c>
+      <c r="R8">
+        <v>19.73</v>
+      </c>
+      <c r="S8">
+        <v>0.125</v>
+      </c>
+      <c r="W8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>92</v>
+      </c>
+      <c r="D9">
+        <v>85</v>
+      </c>
+      <c r="E9">
+        <v>80</v>
+      </c>
+      <c r="F9">
+        <v>65</v>
+      </c>
+      <c r="G9">
+        <v>85</v>
+      </c>
+      <c r="H9">
+        <v>99</v>
+      </c>
+      <c r="J9">
+        <v>99</v>
+      </c>
+      <c r="M9">
+        <v>50</v>
+      </c>
+      <c r="N9">
+        <v>99</v>
+      </c>
+      <c r="Q9">
+        <v>0.125</v>
+      </c>
+      <c r="R9">
+        <v>19.73</v>
+      </c>
+      <c r="S9">
+        <v>0.125</v>
+      </c>
+      <c r="W9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>95</v>
+      </c>
+      <c r="D10">
+        <v>90</v>
+      </c>
+      <c r="E10">
+        <v>88</v>
+      </c>
+      <c r="F10">
+        <v>60</v>
+      </c>
+      <c r="G10">
+        <v>85</v>
+      </c>
+      <c r="H10">
+        <v>99</v>
+      </c>
+      <c r="J10">
+        <v>99</v>
+      </c>
+      <c r="M10">
+        <v>50</v>
+      </c>
+      <c r="N10">
+        <v>99</v>
+      </c>
+      <c r="Q10">
+        <v>0.125</v>
+      </c>
+      <c r="R10">
+        <v>19.73</v>
+      </c>
+      <c r="S10">
+        <v>0.125</v>
+      </c>
+      <c r="W10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>88</v>
+      </c>
+      <c r="D11">
+        <v>85</v>
+      </c>
+      <c r="E11">
+        <v>85</v>
+      </c>
+      <c r="F11">
+        <v>60</v>
+      </c>
+      <c r="G11">
+        <v>85</v>
+      </c>
+      <c r="H11">
+        <v>99</v>
+      </c>
+      <c r="J11">
+        <v>99</v>
+      </c>
+      <c r="M11">
+        <v>45</v>
+      </c>
+      <c r="N11">
+        <v>80</v>
+      </c>
+      <c r="Q11">
+        <v>0.125</v>
+      </c>
+      <c r="R11">
+        <v>19.73</v>
+      </c>
+      <c r="S11">
+        <v>0.125</v>
+      </c>
+      <c r="W11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>88</v>
+      </c>
+      <c r="D12">
+        <v>95</v>
+      </c>
+      <c r="E12">
+        <v>88</v>
+      </c>
+      <c r="F12">
+        <v>50</v>
+      </c>
+      <c r="G12">
+        <v>85</v>
+      </c>
+      <c r="H12">
+        <v>99</v>
+      </c>
+      <c r="J12">
+        <v>99</v>
+      </c>
+      <c r="M12">
+        <v>45</v>
+      </c>
+      <c r="N12">
+        <v>80</v>
+      </c>
+      <c r="Q12">
+        <v>0.125</v>
+      </c>
+      <c r="R12">
+        <v>19.73</v>
+      </c>
+      <c r="S12">
+        <v>0.125</v>
+      </c>
+      <c r="W12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>88</v>
+      </c>
+      <c r="D13">
+        <v>90</v>
+      </c>
+      <c r="E13">
+        <v>85</v>
+      </c>
+      <c r="F13">
+        <v>50</v>
+      </c>
+      <c r="G13">
+        <v>80</v>
+      </c>
+      <c r="H13">
+        <v>99</v>
+      </c>
+      <c r="J13">
+        <v>99</v>
+      </c>
+      <c r="M13">
+        <v>45</v>
+      </c>
+      <c r="N13">
+        <v>80</v>
+      </c>
+      <c r="Q13">
+        <v>0.125</v>
+      </c>
+      <c r="R13">
+        <v>19.73</v>
+      </c>
+      <c r="S13">
+        <v>0.125</v>
+      </c>
+      <c r="W13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>88</v>
+      </c>
+      <c r="D14">
+        <v>87</v>
+      </c>
+      <c r="E14">
+        <v>87</v>
+      </c>
+      <c r="F14">
+        <v>95</v>
+      </c>
+      <c r="G14">
+        <v>80</v>
+      </c>
+      <c r="H14">
+        <v>99</v>
+      </c>
+      <c r="J14">
+        <v>99</v>
+      </c>
+      <c r="M14">
+        <v>45</v>
+      </c>
+      <c r="N14">
+        <v>80</v>
+      </c>
+      <c r="Q14">
+        <v>0.125</v>
+      </c>
+      <c r="R14">
+        <v>19.850000000000001</v>
+      </c>
+      <c r="S14">
+        <v>0.125</v>
+      </c>
+      <c r="W14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>90</v>
+      </c>
+      <c r="D15">
+        <v>97</v>
+      </c>
+      <c r="E15">
+        <v>85</v>
+      </c>
+      <c r="F15">
+        <v>50</v>
+      </c>
+      <c r="G15">
+        <v>75</v>
+      </c>
+      <c r="H15">
+        <v>99</v>
+      </c>
+      <c r="J15">
+        <v>99</v>
+      </c>
+      <c r="M15">
+        <v>45</v>
+      </c>
+      <c r="N15">
+        <v>80</v>
+      </c>
+      <c r="Q15">
+        <v>0.125</v>
+      </c>
+      <c r="R15">
+        <v>19.850000000000001</v>
+      </c>
+      <c r="S15">
+        <v>0.125</v>
+      </c>
+      <c r="W15" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>85</v>
+      </c>
+      <c r="D16">
+        <v>85</v>
+      </c>
+      <c r="E16">
+        <v>85</v>
+      </c>
+      <c r="F16">
+        <v>50</v>
+      </c>
+      <c r="G16">
+        <v>75</v>
+      </c>
+      <c r="H16">
+        <v>99</v>
+      </c>
+      <c r="J16">
+        <v>99</v>
+      </c>
+      <c r="M16">
+        <v>45</v>
+      </c>
+      <c r="N16">
+        <v>70</v>
+      </c>
+      <c r="Q16">
+        <v>0.125</v>
+      </c>
+      <c r="R16">
+        <v>19.850000000000001</v>
+      </c>
+      <c r="S16">
+        <v>0.125</v>
+      </c>
+      <c r="W16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>85</v>
+      </c>
+      <c r="D17">
+        <v>83</v>
+      </c>
+      <c r="E17">
+        <v>85</v>
+      </c>
+      <c r="F17">
+        <v>50</v>
+      </c>
+      <c r="G17">
+        <v>75</v>
+      </c>
+      <c r="H17">
+        <v>99</v>
+      </c>
+      <c r="J17">
+        <v>99</v>
+      </c>
+      <c r="M17">
+        <v>45</v>
+      </c>
+      <c r="N17">
+        <v>70</v>
+      </c>
+      <c r="Q17">
+        <v>0.125</v>
+      </c>
+      <c r="R17">
+        <v>19.850000000000001</v>
+      </c>
+      <c r="S17">
+        <v>0.125</v>
+      </c>
+      <c r="W17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>85</v>
+      </c>
+      <c r="D18">
+        <v>88</v>
+      </c>
+      <c r="E18">
+        <v>85</v>
+      </c>
+      <c r="F18">
+        <v>50</v>
+      </c>
+      <c r="G18">
+        <v>75</v>
+      </c>
+      <c r="H18">
+        <v>99</v>
+      </c>
+      <c r="J18">
+        <v>99</v>
+      </c>
+      <c r="M18">
+        <v>45</v>
+      </c>
+      <c r="N18">
+        <v>65</v>
+      </c>
+      <c r="Q18">
+        <v>0.125</v>
+      </c>
+      <c r="R18">
+        <v>19.850000000000001</v>
+      </c>
+      <c r="S18">
+        <v>0.125</v>
+      </c>
+      <c r="W18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>80</v>
+      </c>
+      <c r="D19">
+        <v>80</v>
+      </c>
+      <c r="E19">
+        <v>80</v>
+      </c>
+      <c r="F19">
+        <v>50</v>
+      </c>
+      <c r="G19">
+        <v>55</v>
+      </c>
+      <c r="H19">
+        <v>99</v>
+      </c>
+      <c r="J19">
+        <v>99</v>
+      </c>
+      <c r="M19">
+        <v>45</v>
+      </c>
+      <c r="N19">
+        <v>65</v>
+      </c>
+      <c r="Q19">
+        <v>0.125</v>
+      </c>
+      <c r="R19">
+        <v>19.850000000000001</v>
+      </c>
+      <c r="S19">
+        <v>0.125</v>
+      </c>
+      <c r="W19" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>80</v>
+      </c>
+      <c r="D20">
+        <v>80</v>
+      </c>
+      <c r="E20">
+        <v>80</v>
+      </c>
+      <c r="F20">
+        <v>50</v>
+      </c>
+      <c r="G20">
+        <v>55</v>
+      </c>
+      <c r="H20">
+        <v>99</v>
+      </c>
+      <c r="J20">
+        <v>99</v>
+      </c>
+      <c r="M20">
+        <v>45</v>
+      </c>
+      <c r="N20">
+        <v>65</v>
+      </c>
+      <c r="Q20">
+        <v>0.125</v>
+      </c>
+      <c r="R20">
+        <v>19.850000000000001</v>
+      </c>
+      <c r="S20">
+        <v>0.125</v>
+      </c>
+      <c r="W20" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>80</v>
+      </c>
+      <c r="D21">
+        <v>80</v>
+      </c>
+      <c r="E21">
+        <v>80</v>
+      </c>
+      <c r="F21">
+        <v>50</v>
+      </c>
+      <c r="G21">
+        <v>55</v>
+      </c>
+      <c r="H21">
+        <v>99</v>
+      </c>
+      <c r="J21">
+        <v>99</v>
+      </c>
+      <c r="M21">
+        <v>45</v>
+      </c>
+      <c r="N21">
+        <v>55</v>
+      </c>
+      <c r="Q21">
+        <v>0.125</v>
+      </c>
+      <c r="R21">
+        <v>19.850000000000001</v>
+      </c>
+      <c r="S21">
+        <v>0.125</v>
+      </c>
+      <c r="W21" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>80</v>
+      </c>
+      <c r="D22">
+        <v>80</v>
+      </c>
+      <c r="E22">
+        <v>80</v>
+      </c>
+      <c r="F22">
+        <v>50</v>
+      </c>
+      <c r="G22">
+        <v>55</v>
+      </c>
+      <c r="H22">
+        <v>99</v>
+      </c>
+      <c r="J22">
+        <v>99</v>
+      </c>
+      <c r="M22">
+        <v>45</v>
+      </c>
+      <c r="N22">
+        <v>50</v>
+      </c>
+      <c r="Q22">
+        <v>0.125</v>
+      </c>
+      <c r="R22">
+        <v>19.850000000000001</v>
+      </c>
+      <c r="S22">
+        <v>0.125</v>
+      </c>
+      <c r="W22" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>90</v>
+      </c>
+      <c r="D23">
+        <v>95</v>
+      </c>
+      <c r="E23">
+        <v>80</v>
+      </c>
+      <c r="F23">
+        <v>50</v>
+      </c>
+      <c r="G23">
+        <v>55</v>
+      </c>
+      <c r="H23">
+        <v>99</v>
+      </c>
+      <c r="J23">
+        <v>99</v>
+      </c>
+      <c r="M23">
+        <v>45</v>
+      </c>
+      <c r="N23">
+        <v>50</v>
+      </c>
+      <c r="Q23">
+        <v>0.125</v>
+      </c>
+      <c r="R23">
+        <v>19.850000000000001</v>
+      </c>
+      <c r="S23">
+        <v>0.125</v>
+      </c>
+      <c r="W23" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>80</v>
+      </c>
+      <c r="D24">
+        <v>80</v>
+      </c>
+      <c r="E24">
+        <v>80</v>
+      </c>
+      <c r="F24">
+        <v>50</v>
+      </c>
+      <c r="G24">
+        <v>55</v>
+      </c>
+      <c r="H24">
+        <v>99</v>
+      </c>
+      <c r="J24">
+        <v>99</v>
+      </c>
+      <c r="M24">
+        <v>45</v>
+      </c>
+      <c r="N24">
+        <v>50</v>
+      </c>
+      <c r="Q24">
+        <v>0.125</v>
+      </c>
+      <c r="R24">
+        <v>19.850000000000001</v>
+      </c>
+      <c r="S24">
+        <v>0.125</v>
+      </c>
+      <c r="W24" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>80</v>
+      </c>
+      <c r="D25">
+        <v>80</v>
+      </c>
+      <c r="E25">
+        <v>80</v>
+      </c>
+      <c r="F25">
+        <v>50</v>
+      </c>
+      <c r="G25">
+        <v>55</v>
+      </c>
+      <c r="H25">
+        <v>99</v>
+      </c>
+      <c r="J25">
+        <v>99</v>
+      </c>
+      <c r="M25">
+        <v>40</v>
+      </c>
+      <c r="N25">
+        <v>50</v>
+      </c>
+      <c r="Q25">
+        <v>0.125</v>
+      </c>
+      <c r="R25">
+        <v>19.93</v>
+      </c>
+      <c r="S25">
+        <v>0.125</v>
+      </c>
+      <c r="W25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>80</v>
+      </c>
+      <c r="D26">
+        <v>80</v>
+      </c>
+      <c r="E26">
+        <v>80</v>
+      </c>
+      <c r="F26">
+        <v>50</v>
+      </c>
+      <c r="G26">
+        <v>45</v>
+      </c>
+      <c r="H26">
+        <v>99</v>
+      </c>
+      <c r="J26">
+        <v>99</v>
+      </c>
+      <c r="M26">
+        <v>40</v>
+      </c>
+      <c r="N26">
+        <v>35</v>
+      </c>
+      <c r="Q26">
+        <v>0.125</v>
+      </c>
+      <c r="R26">
+        <v>19.93</v>
+      </c>
+      <c r="S26">
+        <v>0.125</v>
+      </c>
+      <c r="W26" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>77</v>
+      </c>
+      <c r="D27">
+        <v>75</v>
+      </c>
+      <c r="E27">
+        <v>75</v>
+      </c>
+      <c r="F27">
+        <v>50</v>
+      </c>
+      <c r="G27">
+        <v>45</v>
+      </c>
+      <c r="H27">
+        <v>99</v>
+      </c>
+      <c r="J27">
+        <v>99</v>
+      </c>
+      <c r="M27">
+        <v>40</v>
+      </c>
+      <c r="N27">
+        <v>35</v>
+      </c>
+      <c r="Q27">
+        <v>0.125</v>
+      </c>
+      <c r="R27">
+        <v>19.93</v>
+      </c>
+      <c r="S27">
+        <v>0.125</v>
+      </c>
+      <c r="W27" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>90</v>
+      </c>
+      <c r="D28">
+        <v>75</v>
+      </c>
+      <c r="E28">
+        <v>75</v>
+      </c>
+      <c r="F28">
+        <v>50</v>
+      </c>
+      <c r="G28">
+        <v>45</v>
+      </c>
+      <c r="H28">
+        <v>99</v>
+      </c>
+      <c r="J28">
+        <v>99</v>
+      </c>
+      <c r="M28">
+        <v>40</v>
+      </c>
+      <c r="N28">
+        <v>35</v>
+      </c>
+      <c r="Q28">
+        <v>0.125</v>
+      </c>
+      <c r="R28">
+        <v>19.93</v>
+      </c>
+      <c r="S28">
+        <v>0.125</v>
+      </c>
+      <c r="W28" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>75</v>
+      </c>
+      <c r="D29">
+        <v>75</v>
+      </c>
+      <c r="E29">
+        <v>75</v>
+      </c>
+      <c r="F29">
+        <v>50</v>
+      </c>
+      <c r="G29">
+        <v>45</v>
+      </c>
+      <c r="H29">
+        <v>99</v>
+      </c>
+      <c r="J29">
+        <v>99</v>
+      </c>
+      <c r="M29">
+        <v>40</v>
+      </c>
+      <c r="N29">
+        <v>35</v>
+      </c>
+      <c r="Q29">
+        <v>0.125</v>
+      </c>
+      <c r="R29">
+        <v>19.93</v>
+      </c>
+      <c r="S29">
+        <v>0.125</v>
+      </c>
+      <c r="W29" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>75</v>
+      </c>
+      <c r="D30">
+        <v>75</v>
+      </c>
+      <c r="E30">
+        <v>75</v>
+      </c>
+      <c r="F30">
+        <v>50</v>
+      </c>
+      <c r="G30">
+        <v>45</v>
+      </c>
+      <c r="H30">
+        <v>99</v>
+      </c>
+      <c r="J30">
+        <v>99</v>
+      </c>
+      <c r="M30">
+        <v>40</v>
+      </c>
+      <c r="N30">
+        <v>35</v>
+      </c>
+      <c r="Q30">
+        <v>0.125</v>
+      </c>
+      <c r="R30">
+        <v>19.93</v>
+      </c>
+      <c r="S30">
+        <v>0.125</v>
+      </c>
+      <c r="W30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>72</v>
+      </c>
+      <c r="D31">
+        <v>70</v>
+      </c>
+      <c r="E31">
+        <v>70</v>
+      </c>
+      <c r="F31">
+        <v>50</v>
+      </c>
+      <c r="G31">
+        <v>35</v>
+      </c>
+      <c r="H31">
+        <v>99</v>
+      </c>
+      <c r="J31">
+        <v>99</v>
+      </c>
+      <c r="M31">
+        <v>40</v>
+      </c>
+      <c r="N31">
+        <v>35</v>
+      </c>
+      <c r="Q31">
+        <v>0.125</v>
+      </c>
+      <c r="R31">
+        <v>19.93</v>
+      </c>
+      <c r="S31">
+        <v>0.125</v>
+      </c>
+      <c r="W31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>80</v>
+      </c>
+      <c r="D32">
+        <v>70</v>
+      </c>
+      <c r="E32">
+        <v>70</v>
+      </c>
+      <c r="F32">
+        <v>50</v>
+      </c>
+      <c r="G32">
+        <v>35</v>
+      </c>
+      <c r="H32">
+        <v>99</v>
+      </c>
+      <c r="J32">
+        <v>99</v>
+      </c>
+      <c r="M32">
+        <v>40</v>
+      </c>
+      <c r="N32">
+        <v>35</v>
+      </c>
+      <c r="Q32">
+        <v>0.125</v>
+      </c>
+      <c r="R32">
+        <v>19.93</v>
+      </c>
+      <c r="S32">
+        <v>0.125</v>
+      </c>
+      <c r="W32" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>70</v>
+      </c>
+      <c r="D33">
+        <v>70</v>
+      </c>
+      <c r="E33">
+        <v>70</v>
+      </c>
+      <c r="F33">
+        <v>40</v>
+      </c>
+      <c r="G33">
+        <v>35</v>
+      </c>
+      <c r="H33">
+        <v>99</v>
+      </c>
+      <c r="J33">
+        <v>99</v>
+      </c>
+      <c r="M33">
+        <v>35</v>
+      </c>
+      <c r="N33">
+        <v>35</v>
+      </c>
+      <c r="Q33">
+        <v>0.125</v>
+      </c>
+      <c r="R33">
+        <v>20</v>
+      </c>
+      <c r="S33">
+        <v>0.125</v>
+      </c>
+      <c r="W33" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <v>70</v>
+      </c>
+      <c r="D34">
+        <v>70</v>
+      </c>
+      <c r="E34">
+        <v>70</v>
+      </c>
+      <c r="F34">
+        <v>40</v>
+      </c>
+      <c r="G34">
+        <v>35</v>
+      </c>
+      <c r="H34">
+        <v>99</v>
+      </c>
+      <c r="J34">
+        <v>99</v>
+      </c>
+      <c r="M34">
+        <v>35</v>
+      </c>
+      <c r="N34">
+        <v>35</v>
+      </c>
+      <c r="Q34">
+        <v>0.125</v>
+      </c>
+      <c r="R34">
+        <v>20</v>
+      </c>
+      <c r="S34">
+        <v>0.125</v>
+      </c>
+      <c r="W34" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>70</v>
+      </c>
+      <c r="D35">
+        <v>70</v>
+      </c>
+      <c r="E35">
+        <v>70</v>
+      </c>
+      <c r="F35">
+        <v>40</v>
+      </c>
+      <c r="G35">
+        <v>25</v>
+      </c>
+      <c r="H35">
+        <v>99</v>
+      </c>
+      <c r="J35">
+        <v>99</v>
+      </c>
+      <c r="M35">
+        <v>35</v>
+      </c>
+      <c r="N35">
+        <v>25</v>
+      </c>
+      <c r="Q35">
+        <v>0.125</v>
+      </c>
+      <c r="R35">
+        <v>20</v>
+      </c>
+      <c r="S35">
+        <v>0.125</v>
+      </c>
+      <c r="W35" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36">
+        <v>70</v>
+      </c>
+      <c r="D36">
+        <v>65</v>
+      </c>
+      <c r="E36">
+        <v>65</v>
+      </c>
+      <c r="F36">
+        <v>40</v>
+      </c>
+      <c r="G36">
+        <v>25</v>
+      </c>
+      <c r="H36">
+        <v>99</v>
+      </c>
+      <c r="J36">
+        <v>99</v>
+      </c>
+      <c r="M36">
+        <v>35</v>
+      </c>
+      <c r="N36">
+        <v>25</v>
+      </c>
+      <c r="Q36">
+        <v>0.125</v>
+      </c>
+      <c r="R36">
+        <v>20</v>
+      </c>
+      <c r="S36">
+        <v>0.125</v>
+      </c>
+      <c r="W36" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>75</v>
+      </c>
+      <c r="D37">
+        <v>65</v>
+      </c>
+      <c r="E37">
+        <v>65</v>
+      </c>
+      <c r="F37">
+        <v>40</v>
+      </c>
+      <c r="G37">
+        <v>25</v>
+      </c>
+      <c r="H37">
+        <v>99</v>
+      </c>
+      <c r="J37">
+        <v>99</v>
+      </c>
+      <c r="M37">
+        <v>35</v>
+      </c>
+      <c r="N37">
+        <v>25</v>
+      </c>
+      <c r="Q37">
+        <v>0.125</v>
+      </c>
+      <c r="R37">
+        <v>20</v>
+      </c>
+      <c r="S37">
+        <v>0.125</v>
+      </c>
+      <c r="W37" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <v>75</v>
+      </c>
+      <c r="D38">
+        <v>65</v>
+      </c>
+      <c r="E38">
+        <v>65</v>
+      </c>
+      <c r="F38">
+        <v>40</v>
+      </c>
+      <c r="G38">
+        <v>25</v>
+      </c>
+      <c r="H38">
+        <v>99</v>
+      </c>
+      <c r="J38">
+        <v>99</v>
+      </c>
+      <c r="M38">
+        <v>35</v>
+      </c>
+      <c r="N38">
+        <v>25</v>
+      </c>
+      <c r="Q38">
+        <v>0.125</v>
+      </c>
+      <c r="R38">
+        <v>20</v>
+      </c>
+      <c r="S38">
+        <v>0.125</v>
+      </c>
+      <c r="W38" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <v>72</v>
+      </c>
+      <c r="D39">
+        <v>65</v>
+      </c>
+      <c r="E39">
+        <v>65</v>
+      </c>
+      <c r="F39">
+        <v>35</v>
+      </c>
+      <c r="G39">
+        <v>25</v>
+      </c>
+      <c r="H39">
+        <v>99</v>
+      </c>
+      <c r="J39">
+        <v>99</v>
+      </c>
+      <c r="M39">
+        <v>35</v>
+      </c>
+      <c r="N39">
+        <v>25</v>
+      </c>
+      <c r="Q39">
+        <v>0.125</v>
+      </c>
+      <c r="R39">
+        <v>20</v>
+      </c>
+      <c r="S39">
+        <v>0.125</v>
+      </c>
+      <c r="W39" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40">
+        <v>72</v>
+      </c>
+      <c r="D40">
+        <v>60</v>
+      </c>
+      <c r="E40">
+        <v>60</v>
+      </c>
+      <c r="F40">
+        <v>35</v>
+      </c>
+      <c r="G40">
+        <v>25</v>
+      </c>
+      <c r="H40">
+        <v>99</v>
+      </c>
+      <c r="J40">
+        <v>99</v>
+      </c>
+      <c r="M40">
+        <v>35</v>
+      </c>
+      <c r="N40">
+        <v>25</v>
+      </c>
+      <c r="Q40">
+        <v>0.125</v>
+      </c>
+      <c r="R40">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="S40">
+        <v>0.125</v>
+      </c>
+      <c r="W40" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41">
+        <v>72</v>
+      </c>
+      <c r="D41">
+        <v>60</v>
+      </c>
+      <c r="E41">
+        <v>60</v>
+      </c>
+      <c r="F41">
+        <v>25</v>
+      </c>
+      <c r="G41">
+        <v>25</v>
+      </c>
+      <c r="H41">
+        <v>99</v>
+      </c>
+      <c r="J41">
+        <v>99</v>
+      </c>
+      <c r="M41">
+        <v>35</v>
+      </c>
+      <c r="N41">
+        <v>25</v>
+      </c>
+      <c r="P41">
+        <v>31.2</v>
+      </c>
+      <c r="Q41">
+        <v>0.125</v>
+      </c>
+      <c r="R41">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="S41">
+        <v>0.125</v>
+      </c>
+      <c r="W41" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+      <c r="C42">
+        <v>72</v>
+      </c>
+      <c r="D42">
+        <v>60</v>
+      </c>
+      <c r="E42">
+        <v>60</v>
+      </c>
+      <c r="F42">
+        <v>25</v>
+      </c>
+      <c r="G42">
+        <v>25</v>
+      </c>
+      <c r="H42">
+        <v>99</v>
+      </c>
+      <c r="J42">
+        <v>99</v>
+      </c>
+      <c r="M42">
+        <v>35</v>
+      </c>
+      <c r="N42">
+        <v>25</v>
+      </c>
+      <c r="Q42">
+        <v>0.125</v>
+      </c>
+      <c r="R42">
+        <v>20.2</v>
+      </c>
+      <c r="S42">
+        <v>0.125</v>
+      </c>
+      <c r="W42" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43">
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <v>65</v>
+      </c>
+      <c r="D43">
+        <v>60</v>
+      </c>
+      <c r="E43">
+        <v>60</v>
+      </c>
+      <c r="F43">
+        <v>35</v>
+      </c>
+      <c r="G43">
+        <v>25</v>
+      </c>
+      <c r="H43">
+        <v>99</v>
+      </c>
+      <c r="J43">
+        <v>99</v>
+      </c>
+      <c r="M43">
+        <v>35</v>
+      </c>
+      <c r="N43">
+        <v>25</v>
+      </c>
+      <c r="Q43">
+        <v>0.125</v>
+      </c>
+      <c r="R43">
+        <v>20.2</v>
+      </c>
+      <c r="S43">
+        <v>0.125</v>
+      </c>
+      <c r="W43" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <v>60</v>
+      </c>
+      <c r="D44">
+        <v>55</v>
+      </c>
+      <c r="E44">
+        <v>55</v>
+      </c>
+      <c r="F44">
+        <v>25</v>
+      </c>
+      <c r="G44">
+        <v>15</v>
+      </c>
+      <c r="H44">
+        <v>99</v>
+      </c>
+      <c r="J44">
+        <v>99</v>
+      </c>
+      <c r="M44">
+        <v>35</v>
+      </c>
+      <c r="N44">
+        <v>25</v>
+      </c>
+      <c r="Q44">
+        <v>0.125</v>
+      </c>
+      <c r="R44">
+        <v>20.3</v>
+      </c>
+      <c r="S44">
+        <v>0.125</v>
+      </c>
+      <c r="W44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="C45">
+        <v>55</v>
+      </c>
+      <c r="D45">
+        <v>55</v>
+      </c>
+      <c r="E45">
+        <v>55</v>
+      </c>
+      <c r="F45">
+        <v>25</v>
+      </c>
+      <c r="G45">
+        <v>15</v>
+      </c>
+      <c r="H45">
+        <v>99</v>
+      </c>
+      <c r="J45">
+        <v>99</v>
+      </c>
+      <c r="M45">
+        <v>35</v>
+      </c>
+      <c r="N45">
+        <v>25</v>
+      </c>
+      <c r="Q45">
+        <v>0.125</v>
+      </c>
+      <c r="R45">
+        <v>20.3</v>
+      </c>
+      <c r="S45">
+        <v>0.125</v>
+      </c>
+      <c r="W45" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+      <c r="C46">
+        <v>55</v>
+      </c>
+      <c r="D46">
+        <v>55</v>
+      </c>
+      <c r="E46">
+        <v>55</v>
+      </c>
+      <c r="F46">
+        <v>35</v>
+      </c>
+      <c r="G46">
+        <v>15</v>
+      </c>
+      <c r="H46">
+        <v>99</v>
+      </c>
+      <c r="J46">
+        <v>99</v>
+      </c>
+      <c r="M46">
+        <v>35</v>
+      </c>
+      <c r="N46">
+        <v>25</v>
+      </c>
+      <c r="Q46">
+        <v>0.125</v>
+      </c>
+      <c r="R46">
+        <v>20.3</v>
       </c>
       <c r="S46">
         <v>0.125</v>
@@ -39282,8 +41631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB6F06B3-8EEB-4B02-8F0B-C532C7308BE5}">
   <dimension ref="A1:AB46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updates to add t alent file for new Daytona track
</commit_message>
<xml_diff>
--- a/SCNG2023/SCNG23.xlsx
+++ b/SCNG2023/SCNG23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\rFactor 2\ModDev\Vehicles\SCNG2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EECF90-5657-4223-97E2-1765587BF247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BFB32A-6325-4D09-AE85-BC30160F7FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36780" yWindow="2925" windowWidth="34725" windowHeight="16740" firstSheet="39" activeTab="45" xr2:uid="{EFDCF2A9-BB19-41B3-9ABE-71F143890471}"/>
+    <workbookView xWindow="1620" yWindow="2925" windowWidth="34725" windowHeight="16740" firstSheet="19" activeTab="22" xr2:uid="{EFDCF2A9-BB19-41B3-9ABE-71F143890471}"/>
   </bookViews>
   <sheets>
     <sheet name="Track_Params" sheetId="2" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3447" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3525" uniqueCount="147">
   <si>
     <t>Track</t>
   </si>
@@ -891,7 +891,7 @@
   <dimension ref="A1:T44"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5510,7 +5510,7 @@
   <dimension ref="A1:AB46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17257,9 +17257,11 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4BF095A-4D67-44D3-A924-02D5A6D0FFBE}">
-  <dimension ref="A1:AJ3"/>
+  <dimension ref="A1:AB46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17268,39 +17270,31 @@
     <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>64</v>
       </c>
@@ -17317,178 +17311,2064 @@
         <v>68</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>90</v>
+      </c>
+      <c r="D2">
+        <v>90</v>
+      </c>
+      <c r="E2">
+        <v>90</v>
+      </c>
+      <c r="F2">
         <v>70</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="G2">
+        <v>85</v>
+      </c>
+      <c r="H2">
+        <v>99</v>
+      </c>
+      <c r="J2">
+        <v>99</v>
+      </c>
+      <c r="M2">
+        <v>99</v>
+      </c>
+      <c r="N2">
+        <v>90</v>
+      </c>
+      <c r="Q2">
+        <v>0.125</v>
+      </c>
+      <c r="S2">
+        <v>0.125</v>
+      </c>
+      <c r="W2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>90</v>
+      </c>
+      <c r="D3">
+        <v>90</v>
+      </c>
+      <c r="E3">
+        <v>90</v>
+      </c>
+      <c r="F3">
+        <v>70</v>
+      </c>
+      <c r="G3">
+        <v>90</v>
+      </c>
+      <c r="H3">
+        <v>99</v>
+      </c>
+      <c r="J3">
+        <v>99</v>
+      </c>
+      <c r="M3">
+        <v>97</v>
+      </c>
+      <c r="N3">
+        <v>90</v>
+      </c>
+      <c r="P3">
+        <v>31.2</v>
+      </c>
+      <c r="Q3">
+        <v>0.125</v>
+      </c>
+      <c r="R3">
+        <v>31.2</v>
+      </c>
+      <c r="S3">
+        <v>0.125</v>
+      </c>
+      <c r="W3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>90</v>
+      </c>
+      <c r="D4">
+        <v>88</v>
+      </c>
+      <c r="E4">
+        <v>90</v>
+      </c>
+      <c r="F4">
+        <v>50</v>
+      </c>
+      <c r="G4">
+        <v>85</v>
+      </c>
+      <c r="H4">
+        <v>99</v>
+      </c>
+      <c r="J4">
+        <v>99</v>
+      </c>
+      <c r="M4">
+        <v>95</v>
+      </c>
+      <c r="N4">
+        <v>90</v>
+      </c>
+      <c r="Q4">
+        <v>0.125</v>
+      </c>
+      <c r="S4">
+        <v>0.125</v>
+      </c>
+      <c r="W4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>90</v>
+      </c>
+      <c r="D5">
+        <v>90</v>
+      </c>
+      <c r="E5">
+        <v>85</v>
+      </c>
+      <c r="F5">
+        <v>50</v>
+      </c>
+      <c r="G5">
+        <v>85</v>
+      </c>
+      <c r="H5">
+        <v>99</v>
+      </c>
+      <c r="J5">
+        <v>99</v>
+      </c>
+      <c r="M5">
+        <v>95</v>
+      </c>
+      <c r="N5">
+        <v>87</v>
+      </c>
+      <c r="Q5">
+        <v>0.125</v>
+      </c>
+      <c r="S5">
+        <v>0.125</v>
+      </c>
+      <c r="W5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>90</v>
+      </c>
+      <c r="D6">
+        <v>90</v>
+      </c>
+      <c r="E6">
+        <v>90</v>
+      </c>
+      <c r="F6">
+        <v>50</v>
+      </c>
+      <c r="G6">
+        <v>85</v>
+      </c>
+      <c r="H6">
+        <v>99</v>
+      </c>
+      <c r="J6">
+        <v>99</v>
+      </c>
+      <c r="M6">
+        <v>92</v>
+      </c>
+      <c r="N6">
+        <v>87</v>
+      </c>
+      <c r="Q6">
+        <v>0.125</v>
+      </c>
+      <c r="S6">
+        <v>0.125</v>
+      </c>
+      <c r="W6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>90</v>
+      </c>
+      <c r="D7">
+        <v>90</v>
+      </c>
+      <c r="E7">
+        <v>88</v>
+      </c>
+      <c r="F7">
+        <v>50</v>
+      </c>
+      <c r="G7">
+        <v>85</v>
+      </c>
+      <c r="H7">
+        <v>99</v>
+      </c>
+      <c r="J7">
+        <v>99</v>
+      </c>
+      <c r="M7">
+        <v>95</v>
+      </c>
+      <c r="N7">
+        <v>85</v>
+      </c>
+      <c r="Q7">
+        <v>0.125</v>
+      </c>
+      <c r="S7">
+        <v>0.125</v>
+      </c>
+      <c r="W7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>90</v>
+      </c>
+      <c r="D8">
+        <v>85</v>
+      </c>
+      <c r="E8">
+        <v>90</v>
+      </c>
+      <c r="F8">
+        <v>65</v>
+      </c>
+      <c r="G8">
+        <v>85</v>
+      </c>
+      <c r="H8">
+        <v>99</v>
+      </c>
+      <c r="J8">
+        <v>99</v>
+      </c>
+      <c r="M8">
+        <v>93</v>
+      </c>
+      <c r="N8">
+        <v>82</v>
+      </c>
+      <c r="Q8">
+        <v>0.125</v>
+      </c>
+      <c r="S8">
+        <v>0.125</v>
+      </c>
+      <c r="W8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>90</v>
+      </c>
+      <c r="D9">
+        <v>80</v>
+      </c>
+      <c r="E9">
+        <v>80</v>
+      </c>
+      <c r="F9">
+        <v>50</v>
+      </c>
+      <c r="G9">
+        <v>85</v>
+      </c>
+      <c r="H9">
+        <v>99</v>
+      </c>
+      <c r="J9">
+        <v>99</v>
+      </c>
+      <c r="M9">
+        <v>92</v>
+      </c>
+      <c r="N9">
+        <v>82</v>
+      </c>
+      <c r="Q9">
+        <v>0.125</v>
+      </c>
+      <c r="S9">
+        <v>0.125</v>
+      </c>
+      <c r="W9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>90</v>
+      </c>
+      <c r="D10">
+        <v>90</v>
+      </c>
+      <c r="E10">
+        <v>88</v>
+      </c>
+      <c r="F10">
+        <v>50</v>
+      </c>
+      <c r="G10">
+        <v>85</v>
+      </c>
+      <c r="H10">
+        <v>99</v>
+      </c>
+      <c r="J10">
+        <v>99</v>
+      </c>
+      <c r="M10">
+        <v>90</v>
+      </c>
+      <c r="N10">
+        <v>82</v>
+      </c>
+      <c r="Q10">
+        <v>0.125</v>
+      </c>
+      <c r="S10">
+        <v>0.125</v>
+      </c>
+      <c r="W10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>88</v>
+      </c>
+      <c r="D11">
+        <v>85</v>
+      </c>
+      <c r="E11">
+        <v>85</v>
+      </c>
+      <c r="F11">
+        <v>50</v>
+      </c>
+      <c r="G11">
+        <v>85</v>
+      </c>
+      <c r="H11">
+        <v>99</v>
+      </c>
+      <c r="J11">
+        <v>99</v>
+      </c>
+      <c r="M11">
+        <v>90</v>
+      </c>
+      <c r="N11">
+        <v>80</v>
+      </c>
+      <c r="Q11">
+        <v>0.125</v>
+      </c>
+      <c r="S11">
+        <v>0.125</v>
+      </c>
+      <c r="W11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>88</v>
+      </c>
+      <c r="D12">
+        <v>80</v>
+      </c>
+      <c r="E12">
+        <v>88</v>
+      </c>
+      <c r="F12">
+        <v>50</v>
+      </c>
+      <c r="G12">
+        <v>85</v>
+      </c>
+      <c r="H12">
+        <v>99</v>
+      </c>
+      <c r="J12">
+        <v>99</v>
+      </c>
+      <c r="M12">
+        <v>90</v>
+      </c>
+      <c r="N12">
+        <v>80</v>
+      </c>
+      <c r="Q12">
+        <v>0.125</v>
+      </c>
+      <c r="S12">
+        <v>0.125</v>
+      </c>
+      <c r="W12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>88</v>
+      </c>
+      <c r="D13">
+        <v>88</v>
+      </c>
+      <c r="E13">
+        <v>85</v>
+      </c>
+      <c r="F13">
+        <v>50</v>
+      </c>
+      <c r="G13">
+        <v>80</v>
+      </c>
+      <c r="H13">
+        <v>99</v>
+      </c>
+      <c r="J13">
+        <v>99</v>
+      </c>
+      <c r="M13">
+        <v>90</v>
+      </c>
+      <c r="N13">
+        <v>80</v>
+      </c>
+      <c r="Q13">
+        <v>0.125</v>
+      </c>
+      <c r="S13">
+        <v>0.125</v>
+      </c>
+      <c r="W13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>88</v>
+      </c>
+      <c r="D14">
+        <v>87</v>
+      </c>
+      <c r="E14">
+        <v>87</v>
+      </c>
+      <c r="F14">
+        <v>50</v>
+      </c>
+      <c r="G14">
+        <v>80</v>
+      </c>
+      <c r="H14">
+        <v>99</v>
+      </c>
+      <c r="J14">
+        <v>99</v>
+      </c>
+      <c r="M14">
+        <v>90</v>
+      </c>
+      <c r="N14">
+        <v>80</v>
+      </c>
+      <c r="Q14">
+        <v>0.125</v>
+      </c>
+      <c r="S14">
+        <v>0.125</v>
+      </c>
+      <c r="W14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>85</v>
+      </c>
+      <c r="D15">
+        <v>89</v>
+      </c>
+      <c r="E15">
+        <v>85</v>
+      </c>
+      <c r="F15">
+        <v>50</v>
+      </c>
+      <c r="G15">
+        <v>75</v>
+      </c>
+      <c r="H15">
+        <v>99</v>
+      </c>
+      <c r="J15">
+        <v>99</v>
+      </c>
+      <c r="M15">
+        <v>90</v>
+      </c>
+      <c r="N15">
+        <v>80</v>
+      </c>
+      <c r="Q15">
+        <v>0.125</v>
+      </c>
+      <c r="S15">
+        <v>0.125</v>
+      </c>
+      <c r="W15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>85</v>
+      </c>
+      <c r="D16">
+        <v>85</v>
+      </c>
+      <c r="E16">
+        <v>85</v>
+      </c>
+      <c r="F16">
+        <v>50</v>
+      </c>
+      <c r="G16">
+        <v>75</v>
+      </c>
+      <c r="H16">
+        <v>99</v>
+      </c>
+      <c r="J16">
+        <v>99</v>
+      </c>
+      <c r="M16">
+        <v>90</v>
+      </c>
+      <c r="N16">
+        <v>70</v>
+      </c>
+      <c r="Q16">
+        <v>0.125</v>
+      </c>
+      <c r="S16">
+        <v>0.125</v>
+      </c>
+      <c r="W16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>85</v>
+      </c>
+      <c r="D17">
+        <v>83</v>
+      </c>
+      <c r="E17">
+        <v>85</v>
+      </c>
+      <c r="F17">
+        <v>50</v>
+      </c>
+      <c r="G17">
+        <v>75</v>
+      </c>
+      <c r="H17">
+        <v>99</v>
+      </c>
+      <c r="J17">
+        <v>99</v>
+      </c>
+      <c r="M17">
+        <v>90</v>
+      </c>
+      <c r="N17">
+        <v>70</v>
+      </c>
+      <c r="Q17">
+        <v>0.125</v>
+      </c>
+      <c r="S17">
+        <v>0.125</v>
+      </c>
+      <c r="W17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>85</v>
+      </c>
+      <c r="D18">
+        <v>88</v>
+      </c>
+      <c r="E18">
+        <v>85</v>
+      </c>
+      <c r="F18">
+        <v>50</v>
+      </c>
+      <c r="G18">
+        <v>75</v>
+      </c>
+      <c r="H18">
+        <v>99</v>
+      </c>
+      <c r="J18">
+        <v>99</v>
+      </c>
+      <c r="M18">
+        <v>90</v>
+      </c>
+      <c r="N18">
+        <v>67</v>
+      </c>
+      <c r="Q18">
+        <v>0.125</v>
+      </c>
+      <c r="S18">
+        <v>0.125</v>
+      </c>
+      <c r="W18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>80</v>
+      </c>
+      <c r="D19">
+        <v>80</v>
+      </c>
+      <c r="E19">
+        <v>80</v>
+      </c>
+      <c r="F19">
+        <v>50</v>
+      </c>
+      <c r="G19">
+        <v>75</v>
+      </c>
+      <c r="H19">
+        <v>99</v>
+      </c>
+      <c r="J19">
+        <v>99</v>
+      </c>
+      <c r="M19">
+        <v>90</v>
+      </c>
+      <c r="N19">
+        <v>50</v>
+      </c>
+      <c r="Q19">
+        <v>0.125</v>
+      </c>
+      <c r="S19">
+        <v>0.125</v>
+      </c>
+      <c r="W19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>80</v>
+      </c>
+      <c r="D20">
+        <v>80</v>
+      </c>
+      <c r="E20">
+        <v>80</v>
+      </c>
+      <c r="F20">
+        <v>50</v>
+      </c>
+      <c r="G20">
+        <v>75</v>
+      </c>
+      <c r="H20">
+        <v>99</v>
+      </c>
+      <c r="J20">
+        <v>99</v>
+      </c>
+      <c r="M20">
+        <v>90</v>
+      </c>
+      <c r="N20">
+        <v>50</v>
+      </c>
+      <c r="Q20">
+        <v>0.125</v>
+      </c>
+      <c r="S20">
+        <v>0.125</v>
+      </c>
+      <c r="W20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>80</v>
+      </c>
+      <c r="D21">
+        <v>80</v>
+      </c>
+      <c r="E21">
+        <v>80</v>
+      </c>
+      <c r="F21">
+        <v>50</v>
+      </c>
+      <c r="G21">
+        <v>75</v>
+      </c>
+      <c r="H21">
+        <v>99</v>
+      </c>
+      <c r="J21">
+        <v>99</v>
+      </c>
+      <c r="M21">
+        <v>90</v>
+      </c>
+      <c r="N21">
+        <v>50</v>
+      </c>
+      <c r="Q21">
+        <v>0.125</v>
+      </c>
+      <c r="S21">
+        <v>0.125</v>
+      </c>
+      <c r="W21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>80</v>
+      </c>
+      <c r="D22">
+        <v>80</v>
+      </c>
+      <c r="E22">
+        <v>80</v>
+      </c>
+      <c r="F22">
+        <v>50</v>
+      </c>
+      <c r="G22">
+        <v>75</v>
+      </c>
+      <c r="H22">
+        <v>99</v>
+      </c>
+      <c r="J22">
+        <v>99</v>
+      </c>
+      <c r="M22">
+        <v>90</v>
+      </c>
+      <c r="N22">
+        <v>50</v>
+      </c>
+      <c r="Q22">
+        <v>0.125</v>
+      </c>
+      <c r="S22">
+        <v>0.125</v>
+      </c>
+      <c r="W22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>80</v>
+      </c>
+      <c r="D23">
+        <v>80</v>
+      </c>
+      <c r="E23">
+        <v>80</v>
+      </c>
+      <c r="F23">
+        <v>50</v>
+      </c>
+      <c r="G23">
+        <v>75</v>
+      </c>
+      <c r="H23">
+        <v>99</v>
+      </c>
+      <c r="J23">
+        <v>99</v>
+      </c>
+      <c r="M23">
+        <v>90</v>
+      </c>
+      <c r="N23">
+        <v>50</v>
+      </c>
+      <c r="Q23">
+        <v>0.125</v>
+      </c>
+      <c r="S23">
+        <v>0.125</v>
+      </c>
+      <c r="W23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>80</v>
+      </c>
+      <c r="D24">
+        <v>80</v>
+      </c>
+      <c r="E24">
+        <v>80</v>
+      </c>
+      <c r="F24">
+        <v>50</v>
+      </c>
+      <c r="G24">
+        <v>75</v>
+      </c>
+      <c r="H24">
+        <v>99</v>
+      </c>
+      <c r="J24">
+        <v>99</v>
+      </c>
+      <c r="M24">
+        <v>90</v>
+      </c>
+      <c r="N24">
+        <v>50</v>
+      </c>
+      <c r="Q24">
+        <v>0.125</v>
+      </c>
+      <c r="S24">
+        <v>0.125</v>
+      </c>
+      <c r="W24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>80</v>
+      </c>
+      <c r="D25">
+        <v>80</v>
+      </c>
+      <c r="E25">
+        <v>80</v>
+      </c>
+      <c r="F25">
+        <v>50</v>
+      </c>
+      <c r="G25">
+        <v>75</v>
+      </c>
+      <c r="H25">
+        <v>99</v>
+      </c>
+      <c r="J25">
+        <v>99</v>
+      </c>
+      <c r="M25">
+        <v>90</v>
+      </c>
+      <c r="N25">
+        <v>50</v>
+      </c>
+      <c r="Q25">
+        <v>0.125</v>
+      </c>
+      <c r="S25">
+        <v>0.125</v>
+      </c>
+      <c r="W25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>80</v>
+      </c>
+      <c r="D26">
+        <v>80</v>
+      </c>
+      <c r="E26">
+        <v>80</v>
+      </c>
+      <c r="F26">
+        <v>50</v>
+      </c>
+      <c r="G26">
+        <v>75</v>
+      </c>
+      <c r="H26">
+        <v>99</v>
+      </c>
+      <c r="J26">
+        <v>99</v>
+      </c>
+      <c r="M26">
+        <v>90</v>
+      </c>
+      <c r="N26">
+        <v>50</v>
+      </c>
+      <c r="Q26">
+        <v>0.125</v>
+      </c>
+      <c r="S26">
+        <v>0.125</v>
+      </c>
+      <c r="W26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>77</v>
+      </c>
+      <c r="D27">
+        <v>80</v>
+      </c>
+      <c r="E27">
+        <v>80</v>
+      </c>
+      <c r="F27">
+        <v>50</v>
+      </c>
+      <c r="G27">
+        <v>75</v>
+      </c>
+      <c r="H27">
+        <v>99</v>
+      </c>
+      <c r="J27">
+        <v>99</v>
+      </c>
+      <c r="M27">
+        <v>90</v>
+      </c>
+      <c r="N27">
+        <v>50</v>
+      </c>
+      <c r="Q27">
+        <v>0.125</v>
+      </c>
+      <c r="S27">
+        <v>0.125</v>
+      </c>
+      <c r="W27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>80</v>
+      </c>
+      <c r="D28">
+        <v>80</v>
+      </c>
+      <c r="E28">
+        <v>80</v>
+      </c>
+      <c r="F28">
+        <v>50</v>
+      </c>
+      <c r="G28">
+        <v>75</v>
+      </c>
+      <c r="H28">
+        <v>99</v>
+      </c>
+      <c r="J28">
+        <v>99</v>
+      </c>
+      <c r="M28">
+        <v>90</v>
+      </c>
+      <c r="N28">
+        <v>50</v>
+      </c>
+      <c r="Q28">
+        <v>0.125</v>
+      </c>
+      <c r="S28">
+        <v>0.125</v>
+      </c>
+      <c r="W28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>88</v>
+      </c>
+      <c r="D29">
+        <v>99</v>
+      </c>
+      <c r="E29">
+        <v>80</v>
+      </c>
+      <c r="F29">
+        <v>50</v>
+      </c>
+      <c r="G29">
+        <v>75</v>
+      </c>
+      <c r="H29">
+        <v>99</v>
+      </c>
+      <c r="J29">
+        <v>99</v>
+      </c>
+      <c r="M29">
+        <v>96</v>
+      </c>
+      <c r="N29">
+        <v>75</v>
+      </c>
+      <c r="Q29">
+        <v>0.125</v>
+      </c>
+      <c r="S29">
+        <v>0.125</v>
+      </c>
+      <c r="W29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>88</v>
+      </c>
+      <c r="D30">
+        <v>95</v>
+      </c>
+      <c r="E30">
+        <v>80</v>
+      </c>
+      <c r="F30">
+        <v>50</v>
+      </c>
+      <c r="G30">
+        <v>75</v>
+      </c>
+      <c r="H30">
+        <v>99</v>
+      </c>
+      <c r="J30">
+        <v>99</v>
+      </c>
+      <c r="M30">
+        <v>90</v>
+      </c>
+      <c r="N30">
+        <v>75</v>
+      </c>
+      <c r="Q30">
+        <v>0.125</v>
+      </c>
+      <c r="S30">
+        <v>0.125</v>
+      </c>
+      <c r="W30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>80</v>
+      </c>
+      <c r="D31">
+        <v>80</v>
+      </c>
+      <c r="E31">
+        <v>80</v>
+      </c>
+      <c r="F31">
+        <v>50</v>
+      </c>
+      <c r="G31">
+        <v>75</v>
+      </c>
+      <c r="H31">
+        <v>99</v>
+      </c>
+      <c r="J31">
+        <v>99</v>
+      </c>
+      <c r="M31">
+        <v>90</v>
+      </c>
+      <c r="N31">
+        <v>50</v>
+      </c>
+      <c r="Q31">
+        <v>0.125</v>
+      </c>
+      <c r="S31">
+        <v>0.125</v>
+      </c>
+      <c r="W31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>80</v>
+      </c>
+      <c r="D32">
+        <v>80</v>
+      </c>
+      <c r="E32">
+        <v>80</v>
+      </c>
+      <c r="F32">
+        <v>50</v>
+      </c>
+      <c r="G32">
+        <v>75</v>
+      </c>
+      <c r="H32">
+        <v>99</v>
+      </c>
+      <c r="J32">
+        <v>99</v>
+      </c>
+      <c r="M32">
+        <v>90</v>
+      </c>
+      <c r="N32">
+        <v>50</v>
+      </c>
+      <c r="Q32">
+        <v>0.125</v>
+      </c>
+      <c r="S32">
+        <v>0.125</v>
+      </c>
+      <c r="W32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>80</v>
+      </c>
+      <c r="D33">
+        <v>80</v>
+      </c>
+      <c r="E33">
+        <v>80</v>
+      </c>
+      <c r="F33">
+        <v>50</v>
+      </c>
+      <c r="G33">
+        <v>75</v>
+      </c>
+      <c r="H33">
+        <v>99</v>
+      </c>
+      <c r="J33">
+        <v>99</v>
+      </c>
+      <c r="M33">
+        <v>85</v>
+      </c>
+      <c r="N33">
+        <v>50</v>
+      </c>
+      <c r="Q33">
+        <v>0.125</v>
+      </c>
+      <c r="S33">
+        <v>0.125</v>
+      </c>
+      <c r="W33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <v>80</v>
+      </c>
+      <c r="D34">
+        <v>80</v>
+      </c>
+      <c r="E34">
+        <v>80</v>
+      </c>
+      <c r="F34">
+        <v>50</v>
+      </c>
+      <c r="G34">
+        <v>55</v>
+      </c>
+      <c r="H34">
+        <v>99</v>
+      </c>
+      <c r="J34">
+        <v>99</v>
+      </c>
+      <c r="M34">
+        <v>85</v>
+      </c>
+      <c r="N34">
+        <v>50</v>
+      </c>
+      <c r="Q34">
+        <v>0.125</v>
+      </c>
+      <c r="S34">
+        <v>0.125</v>
+      </c>
+      <c r="W34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>78</v>
+      </c>
+      <c r="D35">
+        <v>80</v>
+      </c>
+      <c r="E35">
+        <v>80</v>
+      </c>
+      <c r="F35">
+        <v>50</v>
+      </c>
+      <c r="G35">
+        <v>55</v>
+      </c>
+      <c r="H35">
+        <v>99</v>
+      </c>
+      <c r="J35">
+        <v>99</v>
+      </c>
+      <c r="M35">
+        <v>85</v>
+      </c>
+      <c r="N35">
+        <v>50</v>
+      </c>
+      <c r="Q35">
+        <v>0.125</v>
+      </c>
+      <c r="S35">
+        <v>0.125</v>
+      </c>
+      <c r="W35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36">
+        <v>77</v>
+      </c>
+      <c r="D36">
+        <v>80</v>
+      </c>
+      <c r="E36">
+        <v>80</v>
+      </c>
+      <c r="F36">
+        <v>50</v>
+      </c>
+      <c r="G36">
+        <v>55</v>
+      </c>
+      <c r="H36">
+        <v>99</v>
+      </c>
+      <c r="J36">
+        <v>99</v>
+      </c>
+      <c r="M36">
+        <v>85</v>
+      </c>
+      <c r="N36">
+        <v>50</v>
+      </c>
+      <c r="Q36">
+        <v>0.125</v>
+      </c>
+      <c r="S36">
+        <v>0.125</v>
+      </c>
+      <c r="W36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>75</v>
+      </c>
+      <c r="D37">
+        <v>80</v>
+      </c>
+      <c r="E37">
+        <v>80</v>
+      </c>
+      <c r="F37">
+        <v>50</v>
+      </c>
+      <c r="G37">
+        <v>55</v>
+      </c>
+      <c r="H37">
+        <v>99</v>
+      </c>
+      <c r="J37">
+        <v>99</v>
+      </c>
+      <c r="M37">
+        <v>85</v>
+      </c>
+      <c r="N37">
+        <v>50</v>
+      </c>
+      <c r="Q37">
+        <v>0.125</v>
+      </c>
+      <c r="S37">
+        <v>0.125</v>
+      </c>
+      <c r="W37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <v>75</v>
+      </c>
+      <c r="D38">
+        <v>70</v>
+      </c>
+      <c r="E38">
+        <v>75</v>
+      </c>
+      <c r="F38">
+        <v>50</v>
+      </c>
+      <c r="G38">
+        <v>55</v>
+      </c>
+      <c r="H38">
+        <v>99</v>
+      </c>
+      <c r="J38">
+        <v>99</v>
+      </c>
+      <c r="M38">
+        <v>85</v>
+      </c>
+      <c r="N38">
+        <v>50</v>
+      </c>
+      <c r="Q38">
+        <v>0.125</v>
+      </c>
+      <c r="S38">
+        <v>0.125</v>
+      </c>
+      <c r="W38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39">
         <v>72</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA1" s="2" t="s">
+      <c r="D39">
+        <v>80</v>
+      </c>
+      <c r="E39">
+        <v>80</v>
+      </c>
+      <c r="F39">
+        <v>40</v>
+      </c>
+      <c r="G39">
+        <v>55</v>
+      </c>
+      <c r="H39">
+        <v>99</v>
+      </c>
+      <c r="J39">
+        <v>99</v>
+      </c>
+      <c r="M39">
+        <v>85</v>
+      </c>
+      <c r="N39">
+        <v>50</v>
+      </c>
+      <c r="Q39">
+        <v>0.125</v>
+      </c>
+      <c r="S39">
+        <v>0.125</v>
+      </c>
+      <c r="W39" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B40">
         <v>4</v>
       </c>
-      <c r="AB1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2">
-        <v>100</v>
-      </c>
-      <c r="D2">
-        <v>100</v>
-      </c>
-      <c r="E2">
-        <v>90</v>
-      </c>
-      <c r="N2">
-        <v>50</v>
-      </c>
-      <c r="O2">
-        <v>50</v>
-      </c>
-      <c r="U2">
-        <v>98</v>
-      </c>
-      <c r="V2">
-        <v>50</v>
-      </c>
-      <c r="X2">
-        <v>49.045000000000002</v>
-      </c>
-      <c r="Y2">
-        <v>0.125</v>
-      </c>
-      <c r="Z2">
-        <v>49.045000000000002</v>
-      </c>
-      <c r="AA2">
-        <v>0.05</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-      <c r="D3">
-        <v>98</v>
-      </c>
-      <c r="E3">
-        <v>90</v>
-      </c>
-      <c r="N3">
-        <v>50</v>
-      </c>
-      <c r="O3">
-        <v>50</v>
-      </c>
-      <c r="U3">
-        <v>98</v>
-      </c>
-      <c r="V3">
-        <v>50</v>
-      </c>
-      <c r="X3">
-        <v>45.314</v>
-      </c>
-      <c r="Y3">
-        <v>0.125</v>
-      </c>
-      <c r="Z3">
-        <v>45.314</v>
-      </c>
-      <c r="AA3">
-        <v>0.05</v>
-      </c>
-      <c r="AE3" t="s">
+      <c r="C40">
+        <v>72</v>
+      </c>
+      <c r="D40">
+        <v>80</v>
+      </c>
+      <c r="E40">
+        <v>80</v>
+      </c>
+      <c r="F40">
+        <v>40</v>
+      </c>
+      <c r="G40">
+        <v>50</v>
+      </c>
+      <c r="H40">
+        <v>99</v>
+      </c>
+      <c r="J40">
+        <v>99</v>
+      </c>
+      <c r="M40">
+        <v>80</v>
+      </c>
+      <c r="N40">
+        <v>50</v>
+      </c>
+      <c r="Q40">
+        <v>0.125</v>
+      </c>
+      <c r="S40">
+        <v>0.125</v>
+      </c>
+      <c r="W40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41">
+        <v>72</v>
+      </c>
+      <c r="D41">
+        <v>80</v>
+      </c>
+      <c r="E41">
+        <v>80</v>
+      </c>
+      <c r="F41">
+        <v>35</v>
+      </c>
+      <c r="G41">
+        <v>45</v>
+      </c>
+      <c r="H41">
+        <v>99</v>
+      </c>
+      <c r="J41">
+        <v>99</v>
+      </c>
+      <c r="M41">
+        <v>80</v>
+      </c>
+      <c r="N41">
+        <v>50</v>
+      </c>
+      <c r="P41">
+        <v>31.2</v>
+      </c>
+      <c r="Q41">
+        <v>0.125</v>
+      </c>
+      <c r="R41">
+        <v>31.3</v>
+      </c>
+      <c r="S41">
+        <v>0.125</v>
+      </c>
+      <c r="W41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+      <c r="C42">
+        <v>72</v>
+      </c>
+      <c r="D42">
+        <v>80</v>
+      </c>
+      <c r="E42">
+        <v>80</v>
+      </c>
+      <c r="F42">
+        <v>35</v>
+      </c>
+      <c r="G42">
+        <v>45</v>
+      </c>
+      <c r="H42">
+        <v>99</v>
+      </c>
+      <c r="J42">
+        <v>99</v>
+      </c>
+      <c r="M42">
+        <v>80</v>
+      </c>
+      <c r="N42">
+        <v>50</v>
+      </c>
+      <c r="Q42">
+        <v>0.125</v>
+      </c>
+      <c r="S42">
+        <v>0.125</v>
+      </c>
+      <c r="W42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43">
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <v>65</v>
+      </c>
+      <c r="D43">
+        <v>60</v>
+      </c>
+      <c r="E43">
+        <v>70</v>
+      </c>
+      <c r="F43">
+        <v>35</v>
+      </c>
+      <c r="G43">
+        <v>45</v>
+      </c>
+      <c r="H43">
+        <v>99</v>
+      </c>
+      <c r="J43">
+        <v>99</v>
+      </c>
+      <c r="M43">
+        <v>75</v>
+      </c>
+      <c r="N43">
+        <v>50</v>
+      </c>
+      <c r="Q43">
+        <v>0.125</v>
+      </c>
+      <c r="S43">
+        <v>0.125</v>
+      </c>
+      <c r="W43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <v>60</v>
+      </c>
+      <c r="D44">
+        <v>70</v>
+      </c>
+      <c r="E44">
+        <v>80</v>
+      </c>
+      <c r="F44">
+        <v>35</v>
+      </c>
+      <c r="G44">
+        <v>35</v>
+      </c>
+      <c r="H44">
+        <v>99</v>
+      </c>
+      <c r="J44">
+        <v>99</v>
+      </c>
+      <c r="M44">
+        <v>75</v>
+      </c>
+      <c r="N44">
+        <v>50</v>
+      </c>
+      <c r="Q44">
+        <v>0.125</v>
+      </c>
+      <c r="S44">
+        <v>0.125</v>
+      </c>
+      <c r="W44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="C45">
+        <v>55</v>
+      </c>
+      <c r="D45">
+        <v>65</v>
+      </c>
+      <c r="E45">
+        <v>80</v>
+      </c>
+      <c r="F45">
+        <v>35</v>
+      </c>
+      <c r="G45">
+        <v>35</v>
+      </c>
+      <c r="H45">
+        <v>99</v>
+      </c>
+      <c r="J45">
+        <v>99</v>
+      </c>
+      <c r="M45">
+        <v>75</v>
+      </c>
+      <c r="N45">
+        <v>50</v>
+      </c>
+      <c r="Q45">
+        <v>0.125</v>
+      </c>
+      <c r="S45">
+        <v>0.125</v>
+      </c>
+      <c r="W45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+      <c r="C46">
+        <v>55</v>
+      </c>
+      <c r="D46">
+        <v>50</v>
+      </c>
+      <c r="E46">
+        <v>80</v>
+      </c>
+      <c r="F46">
+        <v>35</v>
+      </c>
+      <c r="G46">
+        <v>35</v>
+      </c>
+      <c r="H46">
+        <v>99</v>
+      </c>
+      <c r="J46">
+        <v>99</v>
+      </c>
+      <c r="M46">
+        <v>75</v>
+      </c>
+      <c r="N46">
+        <v>50</v>
+      </c>
+      <c r="Q46">
+        <v>0.125</v>
+      </c>
+      <c r="S46">
+        <v>0.125</v>
+      </c>
+      <c r="W46" t="s">
         <v>21</v>
       </c>
     </row>
@@ -42557,7 +44437,7 @@
   <dimension ref="A1:AB46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45322,7 +47202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FE8B38-85A5-4316-9EC1-C52E7892BC51}">
   <dimension ref="A1:AB46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
First cut at michigan
</commit_message>
<xml_diff>
--- a/SCNG2023/SCNG23.xlsx
+++ b/SCNG2023/SCNG23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\rFactor 2\ModDev\Vehicles\SCNG2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC318CF-3643-4C28-9BB8-40131ED532FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6C2253-FB29-4BC3-BF69-AE39CD3144A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33060" yWindow="3795" windowWidth="28800" windowHeight="15435" firstSheet="29" activeTab="33" xr2:uid="{EFDCF2A9-BB19-41B3-9ABE-71F143890471}"/>
+    <workbookView xWindow="-32685" yWindow="3915" windowWidth="28800" windowHeight="15435" xr2:uid="{EFDCF2A9-BB19-41B3-9ABE-71F143890471}"/>
   </bookViews>
   <sheets>
     <sheet name="Track_Params" sheetId="2" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3653" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3693" uniqueCount="148">
   <si>
     <t>Track</t>
   </si>
@@ -894,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50797FCF-F199-4D71-97F5-D5996F6AED8E}">
   <dimension ref="A1:T45"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="Q37" sqref="Q37"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2061,8 +2061,20 @@
       <c r="N24">
         <v>93</v>
       </c>
+      <c r="O24">
+        <v>250</v>
+      </c>
+      <c r="P24">
+        <v>250</v>
+      </c>
+      <c r="Q24">
+        <v>-35</v>
+      </c>
       <c r="R24">
-        <v>10</v>
+        <v>35</v>
+      </c>
+      <c r="S24">
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
@@ -2347,16 +2359,16 @@
         <v>94</v>
       </c>
       <c r="O30">
-        <v>0.1</v>
+        <v>133</v>
       </c>
       <c r="P30">
-        <v>0.1</v>
+        <v>100</v>
       </c>
       <c r="Q30">
-        <v>-36</v>
+        <v>-35</v>
       </c>
       <c r="R30">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="S30">
         <v>1</v>
@@ -2370,16 +2382,22 @@
         <v>49</v>
       </c>
       <c r="O31">
-        <v>0.1</v>
+        <v>133</v>
       </c>
       <c r="P31">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="Q31">
-        <v>100</v>
+        <v>-75</v>
       </c>
       <c r="R31">
-        <v>100</v>
+        <v>25</v>
+      </c>
+      <c r="S31">
+        <v>1</v>
+      </c>
+      <c r="T31" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
@@ -27131,10 +27149,10 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8206A0D4-4DE2-479F-86A5-F72EF3611EA7}">
-  <dimension ref="A1:AJ1"/>
+  <dimension ref="A1:AB46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27144,39 +27162,31 @@
     <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>64</v>
       </c>
@@ -27193,97 +27203,1936 @@
         <v>68</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>99</v>
+      </c>
+      <c r="D2">
+        <v>99</v>
+      </c>
+      <c r="E2">
+        <v>99</v>
+      </c>
+      <c r="F2">
+        <v>95</v>
+      </c>
+      <c r="G2">
+        <v>99</v>
+      </c>
+      <c r="H2">
+        <v>99</v>
+      </c>
+      <c r="J2">
+        <v>99</v>
+      </c>
+      <c r="M2">
+        <v>50</v>
+      </c>
+      <c r="N2">
+        <v>99</v>
+      </c>
+      <c r="Q2">
+        <v>0.125</v>
+      </c>
+      <c r="S2">
+        <v>0.125</v>
+      </c>
+      <c r="W2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>99</v>
+      </c>
+      <c r="D3">
+        <v>99</v>
+      </c>
+      <c r="E3">
+        <v>99</v>
+      </c>
+      <c r="F3">
+        <v>95</v>
+      </c>
+      <c r="G3">
+        <v>99</v>
+      </c>
+      <c r="H3">
+        <v>99</v>
+      </c>
+      <c r="J3">
+        <v>99</v>
+      </c>
+      <c r="M3">
+        <v>50</v>
+      </c>
+      <c r="N3">
+        <v>99</v>
+      </c>
+      <c r="P3">
+        <v>31.2</v>
+      </c>
+      <c r="Q3">
+        <v>0.125</v>
+      </c>
+      <c r="R3">
+        <v>31.2</v>
+      </c>
+      <c r="S3">
+        <v>0.125</v>
+      </c>
+      <c r="W3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>92</v>
+      </c>
+      <c r="D4">
+        <v>88</v>
+      </c>
+      <c r="E4">
+        <v>90</v>
+      </c>
+      <c r="F4">
+        <v>75</v>
+      </c>
+      <c r="G4">
+        <v>85</v>
+      </c>
+      <c r="H4">
+        <v>99</v>
+      </c>
+      <c r="J4">
+        <v>99</v>
+      </c>
+      <c r="M4">
+        <v>50</v>
+      </c>
+      <c r="N4">
+        <v>99</v>
+      </c>
+      <c r="Q4">
+        <v>0.125</v>
+      </c>
+      <c r="S4">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>93</v>
+      </c>
+      <c r="D5">
+        <v>92</v>
+      </c>
+      <c r="E5">
+        <v>85</v>
+      </c>
+      <c r="F5">
+        <v>75</v>
+      </c>
+      <c r="G5">
+        <v>85</v>
+      </c>
+      <c r="H5">
+        <v>99</v>
+      </c>
+      <c r="J5">
+        <v>99</v>
+      </c>
+      <c r="M5">
+        <v>50</v>
+      </c>
+      <c r="N5">
+        <v>99</v>
+      </c>
+      <c r="Q5">
+        <v>0.125</v>
+      </c>
+      <c r="S5">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>95</v>
+      </c>
+      <c r="D6">
+        <v>90</v>
+      </c>
+      <c r="E6">
+        <v>90</v>
+      </c>
+      <c r="F6">
+        <v>80</v>
+      </c>
+      <c r="G6">
+        <v>85</v>
+      </c>
+      <c r="H6">
+        <v>99</v>
+      </c>
+      <c r="J6">
+        <v>99</v>
+      </c>
+      <c r="M6">
+        <v>50</v>
+      </c>
+      <c r="N6">
+        <v>99</v>
+      </c>
+      <c r="Q6">
+        <v>0.125</v>
+      </c>
+      <c r="S6">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>92</v>
+      </c>
+      <c r="D7">
+        <v>91</v>
+      </c>
+      <c r="E7">
+        <v>88</v>
+      </c>
+      <c r="F7">
+        <v>80</v>
+      </c>
+      <c r="G7">
+        <v>85</v>
+      </c>
+      <c r="H7">
+        <v>99</v>
+      </c>
+      <c r="J7">
+        <v>99</v>
+      </c>
+      <c r="M7">
+        <v>50</v>
+      </c>
+      <c r="N7">
+        <v>99</v>
+      </c>
+      <c r="Q7">
+        <v>0.125</v>
+      </c>
+      <c r="S7">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>92</v>
+      </c>
+      <c r="D8">
+        <v>85</v>
+      </c>
+      <c r="E8">
+        <v>90</v>
+      </c>
+      <c r="F8">
+        <v>65</v>
+      </c>
+      <c r="G8">
+        <v>85</v>
+      </c>
+      <c r="H8">
+        <v>99</v>
+      </c>
+      <c r="J8">
+        <v>99</v>
+      </c>
+      <c r="M8">
+        <v>50</v>
+      </c>
+      <c r="N8">
+        <v>99</v>
+      </c>
+      <c r="Q8">
+        <v>0.125</v>
+      </c>
+      <c r="S8">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>92</v>
+      </c>
+      <c r="D9">
+        <v>85</v>
+      </c>
+      <c r="E9">
+        <v>80</v>
+      </c>
+      <c r="F9">
+        <v>65</v>
+      </c>
+      <c r="G9">
+        <v>85</v>
+      </c>
+      <c r="H9">
+        <v>99</v>
+      </c>
+      <c r="J9">
+        <v>99</v>
+      </c>
+      <c r="M9">
+        <v>50</v>
+      </c>
+      <c r="N9">
+        <v>99</v>
+      </c>
+      <c r="Q9">
+        <v>0.125</v>
+      </c>
+      <c r="S9">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>95</v>
+      </c>
+      <c r="D10">
+        <v>90</v>
+      </c>
+      <c r="E10">
+        <v>88</v>
+      </c>
+      <c r="F10">
+        <v>75</v>
+      </c>
+      <c r="G10">
+        <v>85</v>
+      </c>
+      <c r="H10">
+        <v>99</v>
+      </c>
+      <c r="J10">
+        <v>99</v>
+      </c>
+      <c r="M10">
+        <v>50</v>
+      </c>
+      <c r="N10">
+        <v>99</v>
+      </c>
+      <c r="Q10">
+        <v>0.125</v>
+      </c>
+      <c r="S10">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>88</v>
+      </c>
+      <c r="D11">
+        <v>85</v>
+      </c>
+      <c r="E11">
+        <v>85</v>
+      </c>
+      <c r="F11">
+        <v>95</v>
+      </c>
+      <c r="G11">
+        <v>85</v>
+      </c>
+      <c r="H11">
+        <v>99</v>
+      </c>
+      <c r="J11">
+        <v>99</v>
+      </c>
+      <c r="M11">
+        <v>45</v>
+      </c>
+      <c r="N11">
+        <v>80</v>
+      </c>
+      <c r="Q11">
+        <v>0.125</v>
+      </c>
+      <c r="S11">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>88</v>
+      </c>
+      <c r="D12">
+        <v>80</v>
+      </c>
+      <c r="E12">
+        <v>88</v>
+      </c>
+      <c r="F12">
+        <v>50</v>
+      </c>
+      <c r="G12">
+        <v>85</v>
+      </c>
+      <c r="H12">
+        <v>99</v>
+      </c>
+      <c r="J12">
+        <v>99</v>
+      </c>
+      <c r="M12">
+        <v>45</v>
+      </c>
+      <c r="N12">
+        <v>80</v>
+      </c>
+      <c r="Q12">
+        <v>0.125</v>
+      </c>
+      <c r="S12">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>88</v>
+      </c>
+      <c r="D13">
+        <v>88</v>
+      </c>
+      <c r="E13">
+        <v>85</v>
+      </c>
+      <c r="F13">
+        <v>50</v>
+      </c>
+      <c r="G13">
+        <v>80</v>
+      </c>
+      <c r="H13">
+        <v>99</v>
+      </c>
+      <c r="J13">
+        <v>99</v>
+      </c>
+      <c r="M13">
+        <v>45</v>
+      </c>
+      <c r="N13">
+        <v>80</v>
+      </c>
+      <c r="Q13">
+        <v>0.125</v>
+      </c>
+      <c r="S13">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>88</v>
+      </c>
+      <c r="D14">
+        <v>87</v>
+      </c>
+      <c r="E14">
+        <v>87</v>
+      </c>
+      <c r="F14">
+        <v>95</v>
+      </c>
+      <c r="G14">
+        <v>80</v>
+      </c>
+      <c r="H14">
+        <v>99</v>
+      </c>
+      <c r="J14">
+        <v>99</v>
+      </c>
+      <c r="M14">
+        <v>45</v>
+      </c>
+      <c r="N14">
+        <v>80</v>
+      </c>
+      <c r="Q14">
+        <v>0.125</v>
+      </c>
+      <c r="S14">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>85</v>
+      </c>
+      <c r="D15">
+        <v>89</v>
+      </c>
+      <c r="E15">
+        <v>85</v>
+      </c>
+      <c r="F15">
+        <v>50</v>
+      </c>
+      <c r="G15">
+        <v>75</v>
+      </c>
+      <c r="H15">
+        <v>99</v>
+      </c>
+      <c r="J15">
+        <v>99</v>
+      </c>
+      <c r="M15">
+        <v>45</v>
+      </c>
+      <c r="N15">
+        <v>80</v>
+      </c>
+      <c r="Q15">
+        <v>0.125</v>
+      </c>
+      <c r="S15">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>85</v>
+      </c>
+      <c r="D16">
+        <v>85</v>
+      </c>
+      <c r="E16">
+        <v>85</v>
+      </c>
+      <c r="F16">
+        <v>50</v>
+      </c>
+      <c r="G16">
+        <v>75</v>
+      </c>
+      <c r="H16">
+        <v>99</v>
+      </c>
+      <c r="J16">
+        <v>99</v>
+      </c>
+      <c r="M16">
+        <v>45</v>
+      </c>
+      <c r="N16">
         <v>70</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="Q16">
+        <v>0.125</v>
+      </c>
+      <c r="S16">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>85</v>
+      </c>
+      <c r="D17">
+        <v>83</v>
+      </c>
+      <c r="E17">
+        <v>85</v>
+      </c>
+      <c r="F17">
+        <v>50</v>
+      </c>
+      <c r="G17">
+        <v>75</v>
+      </c>
+      <c r="H17">
+        <v>99</v>
+      </c>
+      <c r="J17">
+        <v>99</v>
+      </c>
+      <c r="M17">
+        <v>45</v>
+      </c>
+      <c r="N17">
+        <v>70</v>
+      </c>
+      <c r="Q17">
+        <v>0.125</v>
+      </c>
+      <c r="S17">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>85</v>
+      </c>
+      <c r="D18">
+        <v>88</v>
+      </c>
+      <c r="E18">
+        <v>85</v>
+      </c>
+      <c r="F18">
+        <v>50</v>
+      </c>
+      <c r="G18">
+        <v>75</v>
+      </c>
+      <c r="H18">
+        <v>99</v>
+      </c>
+      <c r="J18">
+        <v>99</v>
+      </c>
+      <c r="M18">
+        <v>45</v>
+      </c>
+      <c r="N18">
+        <v>65</v>
+      </c>
+      <c r="Q18">
+        <v>0.125</v>
+      </c>
+      <c r="S18">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>80</v>
+      </c>
+      <c r="D19">
+        <v>80</v>
+      </c>
+      <c r="E19">
+        <v>80</v>
+      </c>
+      <c r="F19">
+        <v>50</v>
+      </c>
+      <c r="G19">
+        <v>55</v>
+      </c>
+      <c r="H19">
+        <v>99</v>
+      </c>
+      <c r="J19">
+        <v>99</v>
+      </c>
+      <c r="M19">
+        <v>45</v>
+      </c>
+      <c r="N19">
+        <v>65</v>
+      </c>
+      <c r="Q19">
+        <v>0.125</v>
+      </c>
+      <c r="S19">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>80</v>
+      </c>
+      <c r="D20">
+        <v>80</v>
+      </c>
+      <c r="E20">
+        <v>80</v>
+      </c>
+      <c r="F20">
+        <v>50</v>
+      </c>
+      <c r="G20">
+        <v>55</v>
+      </c>
+      <c r="H20">
+        <v>99</v>
+      </c>
+      <c r="J20">
+        <v>99</v>
+      </c>
+      <c r="M20">
+        <v>45</v>
+      </c>
+      <c r="N20">
+        <v>65</v>
+      </c>
+      <c r="Q20">
+        <v>0.125</v>
+      </c>
+      <c r="S20">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>80</v>
+      </c>
+      <c r="D21">
+        <v>80</v>
+      </c>
+      <c r="E21">
+        <v>80</v>
+      </c>
+      <c r="F21">
+        <v>50</v>
+      </c>
+      <c r="G21">
+        <v>55</v>
+      </c>
+      <c r="H21">
+        <v>99</v>
+      </c>
+      <c r="J21">
+        <v>99</v>
+      </c>
+      <c r="M21">
+        <v>45</v>
+      </c>
+      <c r="N21">
+        <v>55</v>
+      </c>
+      <c r="Q21">
+        <v>0.125</v>
+      </c>
+      <c r="S21">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>80</v>
+      </c>
+      <c r="D22">
+        <v>80</v>
+      </c>
+      <c r="E22">
+        <v>80</v>
+      </c>
+      <c r="F22">
+        <v>50</v>
+      </c>
+      <c r="G22">
+        <v>55</v>
+      </c>
+      <c r="H22">
+        <v>99</v>
+      </c>
+      <c r="J22">
+        <v>99</v>
+      </c>
+      <c r="M22">
+        <v>45</v>
+      </c>
+      <c r="N22">
+        <v>50</v>
+      </c>
+      <c r="Q22">
+        <v>0.125</v>
+      </c>
+      <c r="S22">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>80</v>
+      </c>
+      <c r="D23">
+        <v>80</v>
+      </c>
+      <c r="E23">
+        <v>80</v>
+      </c>
+      <c r="F23">
+        <v>50</v>
+      </c>
+      <c r="G23">
+        <v>55</v>
+      </c>
+      <c r="H23">
+        <v>99</v>
+      </c>
+      <c r="J23">
+        <v>99</v>
+      </c>
+      <c r="M23">
+        <v>45</v>
+      </c>
+      <c r="N23">
+        <v>50</v>
+      </c>
+      <c r="Q23">
+        <v>0.125</v>
+      </c>
+      <c r="S23">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>80</v>
+      </c>
+      <c r="D24">
+        <v>80</v>
+      </c>
+      <c r="E24">
+        <v>80</v>
+      </c>
+      <c r="F24">
+        <v>50</v>
+      </c>
+      <c r="G24">
+        <v>55</v>
+      </c>
+      <c r="H24">
+        <v>99</v>
+      </c>
+      <c r="J24">
+        <v>99</v>
+      </c>
+      <c r="M24">
+        <v>45</v>
+      </c>
+      <c r="N24">
+        <v>50</v>
+      </c>
+      <c r="Q24">
+        <v>0.125</v>
+      </c>
+      <c r="S24">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>80</v>
+      </c>
+      <c r="D25">
+        <v>80</v>
+      </c>
+      <c r="E25">
+        <v>80</v>
+      </c>
+      <c r="F25">
+        <v>50</v>
+      </c>
+      <c r="G25">
+        <v>55</v>
+      </c>
+      <c r="H25">
+        <v>99</v>
+      </c>
+      <c r="J25">
+        <v>99</v>
+      </c>
+      <c r="M25">
+        <v>40</v>
+      </c>
+      <c r="N25">
+        <v>50</v>
+      </c>
+      <c r="Q25">
+        <v>0.125</v>
+      </c>
+      <c r="S25">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>80</v>
+      </c>
+      <c r="D26">
+        <v>80</v>
+      </c>
+      <c r="E26">
+        <v>80</v>
+      </c>
+      <c r="F26">
+        <v>50</v>
+      </c>
+      <c r="G26">
+        <v>45</v>
+      </c>
+      <c r="H26">
+        <v>99</v>
+      </c>
+      <c r="J26">
+        <v>99</v>
+      </c>
+      <c r="M26">
+        <v>40</v>
+      </c>
+      <c r="N26">
+        <v>35</v>
+      </c>
+      <c r="Q26">
+        <v>0.125</v>
+      </c>
+      <c r="S26">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>77</v>
+      </c>
+      <c r="D27">
+        <v>75</v>
+      </c>
+      <c r="E27">
+        <v>75</v>
+      </c>
+      <c r="F27">
+        <v>50</v>
+      </c>
+      <c r="G27">
+        <v>45</v>
+      </c>
+      <c r="H27">
+        <v>99</v>
+      </c>
+      <c r="J27">
+        <v>99</v>
+      </c>
+      <c r="M27">
+        <v>40</v>
+      </c>
+      <c r="N27">
+        <v>35</v>
+      </c>
+      <c r="Q27">
+        <v>0.125</v>
+      </c>
+      <c r="S27">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>75</v>
+      </c>
+      <c r="D28">
+        <v>75</v>
+      </c>
+      <c r="E28">
+        <v>75</v>
+      </c>
+      <c r="F28">
+        <v>50</v>
+      </c>
+      <c r="G28">
+        <v>45</v>
+      </c>
+      <c r="H28">
+        <v>99</v>
+      </c>
+      <c r="J28">
+        <v>99</v>
+      </c>
+      <c r="M28">
+        <v>40</v>
+      </c>
+      <c r="N28">
+        <v>35</v>
+      </c>
+      <c r="Q28">
+        <v>0.125</v>
+      </c>
+      <c r="S28">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>75</v>
+      </c>
+      <c r="D29">
+        <v>75</v>
+      </c>
+      <c r="E29">
+        <v>75</v>
+      </c>
+      <c r="F29">
+        <v>50</v>
+      </c>
+      <c r="G29">
+        <v>45</v>
+      </c>
+      <c r="H29">
+        <v>99</v>
+      </c>
+      <c r="J29">
+        <v>99</v>
+      </c>
+      <c r="M29">
+        <v>40</v>
+      </c>
+      <c r="N29">
+        <v>35</v>
+      </c>
+      <c r="Q29">
+        <v>0.125</v>
+      </c>
+      <c r="S29">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>75</v>
+      </c>
+      <c r="D30">
+        <v>75</v>
+      </c>
+      <c r="E30">
+        <v>75</v>
+      </c>
+      <c r="F30">
+        <v>50</v>
+      </c>
+      <c r="G30">
+        <v>45</v>
+      </c>
+      <c r="H30">
+        <v>99</v>
+      </c>
+      <c r="J30">
+        <v>99</v>
+      </c>
+      <c r="M30">
+        <v>40</v>
+      </c>
+      <c r="N30">
+        <v>35</v>
+      </c>
+      <c r="Q30">
+        <v>0.125</v>
+      </c>
+      <c r="S30">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
         <v>72</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z1" s="2" t="s">
+      <c r="D31">
+        <v>70</v>
+      </c>
+      <c r="E31">
+        <v>70</v>
+      </c>
+      <c r="F31">
+        <v>50</v>
+      </c>
+      <c r="G31">
+        <v>35</v>
+      </c>
+      <c r="H31">
+        <v>99</v>
+      </c>
+      <c r="J31">
+        <v>99</v>
+      </c>
+      <c r="M31">
+        <v>40</v>
+      </c>
+      <c r="N31">
+        <v>35</v>
+      </c>
+      <c r="Q31">
+        <v>0.125</v>
+      </c>
+      <c r="S31">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32">
         <v>3</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="C32">
+        <v>80</v>
+      </c>
+      <c r="D32">
+        <v>70</v>
+      </c>
+      <c r="E32">
+        <v>70</v>
+      </c>
+      <c r="F32">
+        <v>50</v>
+      </c>
+      <c r="G32">
+        <v>35</v>
+      </c>
+      <c r="H32">
+        <v>99</v>
+      </c>
+      <c r="J32">
+        <v>99</v>
+      </c>
+      <c r="M32">
+        <v>40</v>
+      </c>
+      <c r="N32">
+        <v>35</v>
+      </c>
+      <c r="Q32">
+        <v>0.125</v>
+      </c>
+      <c r="S32">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33">
         <v>4</v>
       </c>
-      <c r="AB1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>92</v>
+      <c r="C33">
+        <v>70</v>
+      </c>
+      <c r="D33">
+        <v>70</v>
+      </c>
+      <c r="E33">
+        <v>70</v>
+      </c>
+      <c r="F33">
+        <v>40</v>
+      </c>
+      <c r="G33">
+        <v>35</v>
+      </c>
+      <c r="H33">
+        <v>99</v>
+      </c>
+      <c r="J33">
+        <v>99</v>
+      </c>
+      <c r="M33">
+        <v>35</v>
+      </c>
+      <c r="N33">
+        <v>35</v>
+      </c>
+      <c r="Q33">
+        <v>0.125</v>
+      </c>
+      <c r="S33">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <v>70</v>
+      </c>
+      <c r="D34">
+        <v>70</v>
+      </c>
+      <c r="E34">
+        <v>70</v>
+      </c>
+      <c r="F34">
+        <v>40</v>
+      </c>
+      <c r="G34">
+        <v>35</v>
+      </c>
+      <c r="H34">
+        <v>99</v>
+      </c>
+      <c r="J34">
+        <v>99</v>
+      </c>
+      <c r="M34">
+        <v>35</v>
+      </c>
+      <c r="N34">
+        <v>35</v>
+      </c>
+      <c r="Q34">
+        <v>0.125</v>
+      </c>
+      <c r="S34">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>70</v>
+      </c>
+      <c r="D35">
+        <v>70</v>
+      </c>
+      <c r="E35">
+        <v>70</v>
+      </c>
+      <c r="F35">
+        <v>40</v>
+      </c>
+      <c r="G35">
+        <v>25</v>
+      </c>
+      <c r="H35">
+        <v>99</v>
+      </c>
+      <c r="J35">
+        <v>99</v>
+      </c>
+      <c r="M35">
+        <v>35</v>
+      </c>
+      <c r="N35">
+        <v>25</v>
+      </c>
+      <c r="Q35">
+        <v>0.125</v>
+      </c>
+      <c r="S35">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36">
+        <v>70</v>
+      </c>
+      <c r="D36">
+        <v>65</v>
+      </c>
+      <c r="E36">
+        <v>65</v>
+      </c>
+      <c r="F36">
+        <v>40</v>
+      </c>
+      <c r="G36">
+        <v>25</v>
+      </c>
+      <c r="H36">
+        <v>99</v>
+      </c>
+      <c r="J36">
+        <v>99</v>
+      </c>
+      <c r="M36">
+        <v>35</v>
+      </c>
+      <c r="N36">
+        <v>25</v>
+      </c>
+      <c r="Q36">
+        <v>0.125</v>
+      </c>
+      <c r="S36">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>75</v>
+      </c>
+      <c r="D37">
+        <v>65</v>
+      </c>
+      <c r="E37">
+        <v>65</v>
+      </c>
+      <c r="F37">
+        <v>40</v>
+      </c>
+      <c r="G37">
+        <v>25</v>
+      </c>
+      <c r="H37">
+        <v>99</v>
+      </c>
+      <c r="J37">
+        <v>99</v>
+      </c>
+      <c r="M37">
+        <v>35</v>
+      </c>
+      <c r="N37">
+        <v>25</v>
+      </c>
+      <c r="Q37">
+        <v>0.125</v>
+      </c>
+      <c r="S37">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <v>75</v>
+      </c>
+      <c r="D38">
+        <v>65</v>
+      </c>
+      <c r="E38">
+        <v>65</v>
+      </c>
+      <c r="F38">
+        <v>40</v>
+      </c>
+      <c r="G38">
+        <v>25</v>
+      </c>
+      <c r="H38">
+        <v>99</v>
+      </c>
+      <c r="J38">
+        <v>99</v>
+      </c>
+      <c r="M38">
+        <v>35</v>
+      </c>
+      <c r="N38">
+        <v>25</v>
+      </c>
+      <c r="Q38">
+        <v>0.125</v>
+      </c>
+      <c r="S38">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <v>72</v>
+      </c>
+      <c r="D39">
+        <v>65</v>
+      </c>
+      <c r="E39">
+        <v>65</v>
+      </c>
+      <c r="F39">
+        <v>35</v>
+      </c>
+      <c r="G39">
+        <v>25</v>
+      </c>
+      <c r="H39">
+        <v>99</v>
+      </c>
+      <c r="J39">
+        <v>99</v>
+      </c>
+      <c r="M39">
+        <v>35</v>
+      </c>
+      <c r="N39">
+        <v>25</v>
+      </c>
+      <c r="Q39">
+        <v>0.125</v>
+      </c>
+      <c r="S39">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40">
+        <v>72</v>
+      </c>
+      <c r="D40">
+        <v>60</v>
+      </c>
+      <c r="E40">
+        <v>60</v>
+      </c>
+      <c r="F40">
+        <v>35</v>
+      </c>
+      <c r="G40">
+        <v>25</v>
+      </c>
+      <c r="H40">
+        <v>99</v>
+      </c>
+      <c r="J40">
+        <v>99</v>
+      </c>
+      <c r="M40">
+        <v>35</v>
+      </c>
+      <c r="N40">
+        <v>25</v>
+      </c>
+      <c r="Q40">
+        <v>0.125</v>
+      </c>
+      <c r="S40">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41">
+        <v>72</v>
+      </c>
+      <c r="D41">
+        <v>60</v>
+      </c>
+      <c r="E41">
+        <v>60</v>
+      </c>
+      <c r="F41">
+        <v>25</v>
+      </c>
+      <c r="G41">
+        <v>25</v>
+      </c>
+      <c r="H41">
+        <v>99</v>
+      </c>
+      <c r="J41">
+        <v>99</v>
+      </c>
+      <c r="M41">
+        <v>35</v>
+      </c>
+      <c r="N41">
+        <v>25</v>
+      </c>
+      <c r="P41">
+        <v>31.2</v>
+      </c>
+      <c r="Q41">
+        <v>0.125</v>
+      </c>
+      <c r="R41">
+        <v>31.3</v>
+      </c>
+      <c r="S41">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+      <c r="C42">
+        <v>72</v>
+      </c>
+      <c r="D42">
+        <v>60</v>
+      </c>
+      <c r="E42">
+        <v>60</v>
+      </c>
+      <c r="F42">
+        <v>25</v>
+      </c>
+      <c r="G42">
+        <v>25</v>
+      </c>
+      <c r="H42">
+        <v>99</v>
+      </c>
+      <c r="J42">
+        <v>99</v>
+      </c>
+      <c r="M42">
+        <v>35</v>
+      </c>
+      <c r="N42">
+        <v>25</v>
+      </c>
+      <c r="Q42">
+        <v>0.125</v>
+      </c>
+      <c r="S42">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43">
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <v>65</v>
+      </c>
+      <c r="D43">
+        <v>60</v>
+      </c>
+      <c r="E43">
+        <v>60</v>
+      </c>
+      <c r="F43">
+        <v>35</v>
+      </c>
+      <c r="G43">
+        <v>25</v>
+      </c>
+      <c r="H43">
+        <v>99</v>
+      </c>
+      <c r="J43">
+        <v>99</v>
+      </c>
+      <c r="M43">
+        <v>35</v>
+      </c>
+      <c r="N43">
+        <v>25</v>
+      </c>
+      <c r="Q43">
+        <v>0.125</v>
+      </c>
+      <c r="S43">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <v>60</v>
+      </c>
+      <c r="D44">
+        <v>55</v>
+      </c>
+      <c r="E44">
+        <v>55</v>
+      </c>
+      <c r="F44">
+        <v>25</v>
+      </c>
+      <c r="G44">
+        <v>15</v>
+      </c>
+      <c r="H44">
+        <v>99</v>
+      </c>
+      <c r="J44">
+        <v>99</v>
+      </c>
+      <c r="M44">
+        <v>35</v>
+      </c>
+      <c r="N44">
+        <v>25</v>
+      </c>
+      <c r="Q44">
+        <v>0.125</v>
+      </c>
+      <c r="S44">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="C45">
+        <v>55</v>
+      </c>
+      <c r="D45">
+        <v>55</v>
+      </c>
+      <c r="E45">
+        <v>55</v>
+      </c>
+      <c r="F45">
+        <v>25</v>
+      </c>
+      <c r="G45">
+        <v>15</v>
+      </c>
+      <c r="H45">
+        <v>99</v>
+      </c>
+      <c r="J45">
+        <v>99</v>
+      </c>
+      <c r="M45">
+        <v>35</v>
+      </c>
+      <c r="N45">
+        <v>25</v>
+      </c>
+      <c r="Q45">
+        <v>0.125</v>
+      </c>
+      <c r="S45">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+      <c r="C46">
+        <v>55</v>
+      </c>
+      <c r="D46">
+        <v>55</v>
+      </c>
+      <c r="E46">
+        <v>55</v>
+      </c>
+      <c r="F46">
+        <v>35</v>
+      </c>
+      <c r="G46">
+        <v>15</v>
+      </c>
+      <c r="H46">
+        <v>99</v>
+      </c>
+      <c r="J46">
+        <v>99</v>
+      </c>
+      <c r="M46">
+        <v>35</v>
+      </c>
+      <c r="N46">
+        <v>25</v>
+      </c>
+      <c r="Q46">
+        <v>0.125</v>
+      </c>
+      <c r="S46">
+        <v>0.125</v>
       </c>
     </row>
   </sheetData>
@@ -27296,7 +29145,7 @@
   <dimension ref="A1:AB46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T52" sqref="T52"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31398,7 +33247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B82838E6-E76B-4E38-AA30-68C94895E3CF}">
   <dimension ref="A1:AB46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>

</xml_diff>